<commit_message>
Remove year 2051 to 2100 for lifetime
</commit_message>
<xml_diff>
--- a/Data/regression_data/Dwelling_Lifetime/regression_Dwelling_Lifetime.xlsx
+++ b/Data/regression_data/Dwelling_Lifetime/regression_Dwelling_Lifetime.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D502"/>
+  <dimension ref="A1:D452"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,10 +458,10 @@
         <v>1600</v>
       </c>
       <c r="C2" t="n">
-        <v>186.6666666666666</v>
+        <v>186.6666666666667</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3666666666666666</v>
+        <v>0.3666666666666667</v>
       </c>
     </row>
     <row r="3">
@@ -472,10 +472,10 @@
         <v>1601</v>
       </c>
       <c r="C3" t="n">
-        <v>186.4833333333332</v>
+        <v>186.4833333333333</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3663333333333333</v>
+        <v>0.3663333333333334</v>
       </c>
     </row>
     <row r="4">
@@ -486,10 +486,10 @@
         <v>1602</v>
       </c>
       <c r="C4" t="n">
-        <v>186.2999999999999</v>
+        <v>186.3</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3659999999999999</v>
+        <v>0.3660000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -500,10 +500,10 @@
         <v>1603</v>
       </c>
       <c r="C5" t="n">
-        <v>186.1166666666666</v>
+        <v>186.1166666666667</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3656666666666666</v>
+        <v>0.3656666666666667</v>
       </c>
     </row>
     <row r="6">
@@ -514,10 +514,10 @@
         <v>1604</v>
       </c>
       <c r="C6" t="n">
-        <v>185.9333333333332</v>
+        <v>185.9333333333333</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3653333333333333</v>
+        <v>0.3653333333333334</v>
       </c>
     </row>
     <row r="7">
@@ -528,10 +528,10 @@
         <v>1605</v>
       </c>
       <c r="C7" t="n">
-        <v>185.7499999999999</v>
+        <v>185.75</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3649999999999999</v>
+        <v>0.3650000000000001</v>
       </c>
     </row>
     <row r="8">
@@ -542,10 +542,10 @@
         <v>1606</v>
       </c>
       <c r="C8" t="n">
-        <v>185.5666666666665</v>
+        <v>185.5666666666667</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3646666666666666</v>
+        <v>0.3646666666666667</v>
       </c>
     </row>
     <row r="9">
@@ -556,10 +556,10 @@
         <v>1607</v>
       </c>
       <c r="C9" t="n">
-        <v>185.3833333333332</v>
+        <v>185.3833333333333</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3643333333333333</v>
+        <v>0.3643333333333334</v>
       </c>
     </row>
     <row r="10">
@@ -570,10 +570,10 @@
         <v>1608</v>
       </c>
       <c r="C10" t="n">
-        <v>185.1999999999999</v>
+        <v>185.2</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3639999999999999</v>
+        <v>0.3640000000000001</v>
       </c>
     </row>
     <row r="11">
@@ -584,10 +584,10 @@
         <v>1609</v>
       </c>
       <c r="C11" t="n">
-        <v>185.0166666666665</v>
+        <v>185.0166666666667</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3636666666666666</v>
+        <v>0.3636666666666667</v>
       </c>
     </row>
     <row r="12">
@@ -598,10 +598,10 @@
         <v>1610</v>
       </c>
       <c r="C12" t="n">
-        <v>184.8333333333333</v>
+        <v>184.8333333333334</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3633333333333333</v>
+        <v>0.3633333333333334</v>
       </c>
     </row>
     <row r="13">
@@ -612,10 +612,10 @@
         <v>1611</v>
       </c>
       <c r="C13" t="n">
-        <v>184.6499999999999</v>
+        <v>184.65</v>
       </c>
       <c r="D13" t="n">
-        <v>0.3629999999999999</v>
+        <v>0.3630000000000001</v>
       </c>
     </row>
     <row r="14">
@@ -626,10 +626,10 @@
         <v>1612</v>
       </c>
       <c r="C14" t="n">
-        <v>184.4666666666666</v>
+        <v>184.4666666666667</v>
       </c>
       <c r="D14" t="n">
-        <v>0.3626666666666666</v>
+        <v>0.3626666666666667</v>
       </c>
     </row>
     <row r="15">
@@ -640,10 +640,10 @@
         <v>1613</v>
       </c>
       <c r="C15" t="n">
-        <v>184.2833333333332</v>
+        <v>184.2833333333334</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3623333333333333</v>
+        <v>0.3623333333333334</v>
       </c>
     </row>
     <row r="16">
@@ -654,10 +654,10 @@
         <v>1614</v>
       </c>
       <c r="C16" t="n">
-        <v>184.0999999999999</v>
+        <v>184.1</v>
       </c>
       <c r="D16" t="n">
-        <v>0.3619999999999999</v>
+        <v>0.3620000000000001</v>
       </c>
     </row>
     <row r="17">
@@ -668,10 +668,10 @@
         <v>1615</v>
       </c>
       <c r="C17" t="n">
-        <v>183.9166666666666</v>
+        <v>183.9166666666667</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3616666666666666</v>
+        <v>0.3616666666666668</v>
       </c>
     </row>
     <row r="18">
@@ -682,10 +682,10 @@
         <v>1616</v>
       </c>
       <c r="C18" t="n">
-        <v>183.7333333333332</v>
+        <v>183.7333333333333</v>
       </c>
       <c r="D18" t="n">
-        <v>0.3613333333333333</v>
+        <v>0.3613333333333334</v>
       </c>
     </row>
     <row r="19">
@@ -696,10 +696,10 @@
         <v>1617</v>
       </c>
       <c r="C19" t="n">
-        <v>183.5499999999999</v>
+        <v>183.55</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3609999999999999</v>
+        <v>0.3610000000000001</v>
       </c>
     </row>
     <row r="20">
@@ -710,10 +710,10 @@
         <v>1618</v>
       </c>
       <c r="C20" t="n">
-        <v>183.3666666666666</v>
+        <v>183.3666666666667</v>
       </c>
       <c r="D20" t="n">
-        <v>0.3606666666666666</v>
+        <v>0.3606666666666668</v>
       </c>
     </row>
     <row r="21">
@@ -724,10 +724,10 @@
         <v>1619</v>
       </c>
       <c r="C21" t="n">
-        <v>183.1833333333332</v>
+        <v>183.1833333333333</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3603333333333333</v>
+        <v>0.3603333333333334</v>
       </c>
     </row>
     <row r="22">
@@ -738,10 +738,10 @@
         <v>1620</v>
       </c>
       <c r="C22" t="n">
-        <v>182.9999999999999</v>
+        <v>183</v>
       </c>
       <c r="D22" t="n">
-        <v>0.3599999999999999</v>
+        <v>0.3600000000000001</v>
       </c>
     </row>
     <row r="23">
@@ -752,10 +752,10 @@
         <v>1621</v>
       </c>
       <c r="C23" t="n">
-        <v>182.8166666666665</v>
+        <v>182.8166666666667</v>
       </c>
       <c r="D23" t="n">
-        <v>0.3596666666666666</v>
+        <v>0.3596666666666668</v>
       </c>
     </row>
     <row r="24">
@@ -766,10 +766,10 @@
         <v>1622</v>
       </c>
       <c r="C24" t="n">
-        <v>182.6333333333332</v>
+        <v>182.6333333333333</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3593333333333333</v>
+        <v>0.3593333333333334</v>
       </c>
     </row>
     <row r="25">
@@ -780,10 +780,10 @@
         <v>1623</v>
       </c>
       <c r="C25" t="n">
-        <v>182.4499999999999</v>
+        <v>182.45</v>
       </c>
       <c r="D25" t="n">
-        <v>0.3589999999999999</v>
+        <v>0.3590000000000001</v>
       </c>
     </row>
     <row r="26">
@@ -794,10 +794,10 @@
         <v>1624</v>
       </c>
       <c r="C26" t="n">
-        <v>182.2666666666666</v>
+        <v>182.2666666666667</v>
       </c>
       <c r="D26" t="n">
-        <v>0.3586666666666666</v>
+        <v>0.3586666666666668</v>
       </c>
     </row>
     <row r="27">
@@ -808,10 +808,10 @@
         <v>1625</v>
       </c>
       <c r="C27" t="n">
-        <v>182.0833333333333</v>
+        <v>182.0833333333334</v>
       </c>
       <c r="D27" t="n">
-        <v>0.3583333333333333</v>
+        <v>0.3583333333333334</v>
       </c>
     </row>
     <row r="28">
@@ -822,10 +822,10 @@
         <v>1626</v>
       </c>
       <c r="C28" t="n">
-        <v>181.8999999999999</v>
+        <v>181.9</v>
       </c>
       <c r="D28" t="n">
-        <v>0.3579999999999999</v>
+        <v>0.3580000000000001</v>
       </c>
     </row>
     <row r="29">
@@ -836,10 +836,10 @@
         <v>1627</v>
       </c>
       <c r="C29" t="n">
-        <v>181.7166666666666</v>
+        <v>181.7166666666667</v>
       </c>
       <c r="D29" t="n">
-        <v>0.3576666666666666</v>
+        <v>0.3576666666666668</v>
       </c>
     </row>
     <row r="30">
@@ -850,10 +850,10 @@
         <v>1628</v>
       </c>
       <c r="C30" t="n">
-        <v>181.5333333333332</v>
+        <v>181.5333333333334</v>
       </c>
       <c r="D30" t="n">
-        <v>0.3573333333333333</v>
+        <v>0.3573333333333334</v>
       </c>
     </row>
     <row r="31">
@@ -864,10 +864,10 @@
         <v>1629</v>
       </c>
       <c r="C31" t="n">
-        <v>181.3499999999999</v>
+        <v>181.35</v>
       </c>
       <c r="D31" t="n">
-        <v>0.3569999999999999</v>
+        <v>0.3570000000000001</v>
       </c>
     </row>
     <row r="32">
@@ -878,10 +878,10 @@
         <v>1630</v>
       </c>
       <c r="C32" t="n">
-        <v>181.1666666666666</v>
+        <v>181.1666666666667</v>
       </c>
       <c r="D32" t="n">
-        <v>0.3566666666666666</v>
+        <v>0.3566666666666668</v>
       </c>
     </row>
     <row r="33">
@@ -892,10 +892,10 @@
         <v>1631</v>
       </c>
       <c r="C33" t="n">
-        <v>180.9833333333332</v>
+        <v>180.9833333333333</v>
       </c>
       <c r="D33" t="n">
-        <v>0.3563333333333333</v>
+        <v>0.3563333333333334</v>
       </c>
     </row>
     <row r="34">
@@ -906,10 +906,10 @@
         <v>1632</v>
       </c>
       <c r="C34" t="n">
-        <v>180.7999999999999</v>
+        <v>180.8</v>
       </c>
       <c r="D34" t="n">
-        <v>0.3559999999999999</v>
+        <v>0.3560000000000001</v>
       </c>
     </row>
     <row r="35">
@@ -920,10 +920,10 @@
         <v>1633</v>
       </c>
       <c r="C35" t="n">
-        <v>180.6166666666666</v>
+        <v>180.6166666666667</v>
       </c>
       <c r="D35" t="n">
-        <v>0.3556666666666666</v>
+        <v>0.3556666666666668</v>
       </c>
     </row>
     <row r="36">
@@ -934,10 +934,10 @@
         <v>1634</v>
       </c>
       <c r="C36" t="n">
-        <v>180.4333333333332</v>
+        <v>180.4333333333333</v>
       </c>
       <c r="D36" t="n">
-        <v>0.3553333333333333</v>
+        <v>0.3553333333333334</v>
       </c>
     </row>
     <row r="37">
@@ -948,10 +948,10 @@
         <v>1635</v>
       </c>
       <c r="C37" t="n">
-        <v>180.2499999999999</v>
+        <v>180.25</v>
       </c>
       <c r="D37" t="n">
-        <v>0.355</v>
+        <v>0.3550000000000001</v>
       </c>
     </row>
     <row r="38">
@@ -962,10 +962,10 @@
         <v>1636</v>
       </c>
       <c r="C38" t="n">
-        <v>180.0666666666665</v>
+        <v>180.0666666666667</v>
       </c>
       <c r="D38" t="n">
-        <v>0.3546666666666666</v>
+        <v>0.3546666666666668</v>
       </c>
     </row>
     <row r="39">
@@ -976,10 +976,10 @@
         <v>1637</v>
       </c>
       <c r="C39" t="n">
-        <v>179.8833333333332</v>
+        <v>179.8833333333333</v>
       </c>
       <c r="D39" t="n">
-        <v>0.3543333333333333</v>
+        <v>0.3543333333333334</v>
       </c>
     </row>
     <row r="40">
@@ -990,10 +990,10 @@
         <v>1638</v>
       </c>
       <c r="C40" t="n">
-        <v>179.6999999999999</v>
+        <v>179.7</v>
       </c>
       <c r="D40" t="n">
-        <v>0.354</v>
+        <v>0.3540000000000001</v>
       </c>
     </row>
     <row r="41">
@@ -1004,10 +1004,10 @@
         <v>1639</v>
       </c>
       <c r="C41" t="n">
-        <v>179.5166666666666</v>
+        <v>179.5166666666667</v>
       </c>
       <c r="D41" t="n">
-        <v>0.3536666666666666</v>
+        <v>0.3536666666666668</v>
       </c>
     </row>
     <row r="42">
@@ -1018,10 +1018,10 @@
         <v>1640</v>
       </c>
       <c r="C42" t="n">
-        <v>179.3333333333333</v>
+        <v>179.3333333333334</v>
       </c>
       <c r="D42" t="n">
-        <v>0.3533333333333333</v>
+        <v>0.3533333333333334</v>
       </c>
     </row>
     <row r="43">
@@ -1032,10 +1032,10 @@
         <v>1641</v>
       </c>
       <c r="C43" t="n">
-        <v>179.1499999999999</v>
+        <v>179.15</v>
       </c>
       <c r="D43" t="n">
-        <v>0.353</v>
+        <v>0.3530000000000001</v>
       </c>
     </row>
     <row r="44">
@@ -1046,10 +1046,10 @@
         <v>1642</v>
       </c>
       <c r="C44" t="n">
-        <v>178.9666666666666</v>
+        <v>178.9666666666667</v>
       </c>
       <c r="D44" t="n">
-        <v>0.3526666666666666</v>
+        <v>0.3526666666666668</v>
       </c>
     </row>
     <row r="45">
@@ -1060,10 +1060,10 @@
         <v>1643</v>
       </c>
       <c r="C45" t="n">
-        <v>178.7833333333332</v>
+        <v>178.7833333333334</v>
       </c>
       <c r="D45" t="n">
-        <v>0.3523333333333333</v>
+        <v>0.3523333333333334</v>
       </c>
     </row>
     <row r="46">
@@ -1074,10 +1074,10 @@
         <v>1644</v>
       </c>
       <c r="C46" t="n">
-        <v>178.5999999999999</v>
+        <v>178.6</v>
       </c>
       <c r="D46" t="n">
-        <v>0.352</v>
+        <v>0.3520000000000001</v>
       </c>
     </row>
     <row r="47">
@@ -1088,10 +1088,10 @@
         <v>1645</v>
       </c>
       <c r="C47" t="n">
-        <v>178.4166666666666</v>
+        <v>178.4166666666667</v>
       </c>
       <c r="D47" t="n">
-        <v>0.3516666666666666</v>
+        <v>0.3516666666666668</v>
       </c>
     </row>
     <row r="48">
@@ -1102,10 +1102,10 @@
         <v>1646</v>
       </c>
       <c r="C48" t="n">
-        <v>178.2333333333332</v>
+        <v>178.2333333333333</v>
       </c>
       <c r="D48" t="n">
-        <v>0.3513333333333333</v>
+        <v>0.3513333333333334</v>
       </c>
     </row>
     <row r="49">
@@ -1116,10 +1116,10 @@
         <v>1647</v>
       </c>
       <c r="C49" t="n">
-        <v>178.0499999999999</v>
+        <v>178.05</v>
       </c>
       <c r="D49" t="n">
-        <v>0.351</v>
+        <v>0.3510000000000001</v>
       </c>
     </row>
     <row r="50">
@@ -1130,10 +1130,10 @@
         <v>1648</v>
       </c>
       <c r="C50" t="n">
-        <v>177.8666666666666</v>
+        <v>177.8666666666667</v>
       </c>
       <c r="D50" t="n">
-        <v>0.3506666666666666</v>
+        <v>0.3506666666666668</v>
       </c>
     </row>
     <row r="51">
@@ -1144,10 +1144,10 @@
         <v>1649</v>
       </c>
       <c r="C51" t="n">
-        <v>177.6833333333332</v>
+        <v>177.6833333333333</v>
       </c>
       <c r="D51" t="n">
-        <v>0.3503333333333333</v>
+        <v>0.3503333333333334</v>
       </c>
     </row>
     <row r="52">
@@ -1158,10 +1158,10 @@
         <v>1650</v>
       </c>
       <c r="C52" t="n">
-        <v>177.4999999999999</v>
+        <v>177.5</v>
       </c>
       <c r="D52" t="n">
-        <v>0.35</v>
+        <v>0.3500000000000001</v>
       </c>
     </row>
     <row r="53">
@@ -1172,10 +1172,10 @@
         <v>1651</v>
       </c>
       <c r="C53" t="n">
-        <v>177.3166666666666</v>
+        <v>177.3166666666667</v>
       </c>
       <c r="D53" t="n">
-        <v>0.3496666666666666</v>
+        <v>0.3496666666666668</v>
       </c>
     </row>
     <row r="54">
@@ -1186,10 +1186,10 @@
         <v>1652</v>
       </c>
       <c r="C54" t="n">
-        <v>177.1333333333333</v>
+        <v>177.1333333333334</v>
       </c>
       <c r="D54" t="n">
-        <v>0.3493333333333333</v>
+        <v>0.3493333333333334</v>
       </c>
     </row>
     <row r="55">
@@ -1200,10 +1200,10 @@
         <v>1653</v>
       </c>
       <c r="C55" t="n">
-        <v>176.9499999999999</v>
+        <v>176.95</v>
       </c>
       <c r="D55" t="n">
-        <v>0.349</v>
+        <v>0.3490000000000001</v>
       </c>
     </row>
     <row r="56">
@@ -1214,10 +1214,10 @@
         <v>1654</v>
       </c>
       <c r="C56" t="n">
-        <v>176.7666666666666</v>
+        <v>176.7666666666667</v>
       </c>
       <c r="D56" t="n">
-        <v>0.3486666666666666</v>
+        <v>0.3486666666666668</v>
       </c>
     </row>
     <row r="57">
@@ -1228,10 +1228,10 @@
         <v>1655</v>
       </c>
       <c r="C57" t="n">
-        <v>176.5833333333333</v>
+        <v>176.5833333333334</v>
       </c>
       <c r="D57" t="n">
-        <v>0.3483333333333333</v>
+        <v>0.3483333333333334</v>
       </c>
     </row>
     <row r="58">
@@ -1242,10 +1242,10 @@
         <v>1656</v>
       </c>
       <c r="C58" t="n">
-        <v>176.3999999999999</v>
+        <v>176.4</v>
       </c>
       <c r="D58" t="n">
-        <v>0.348</v>
+        <v>0.3480000000000001</v>
       </c>
     </row>
     <row r="59">
@@ -1256,10 +1256,10 @@
         <v>1657</v>
       </c>
       <c r="C59" t="n">
-        <v>176.2166666666666</v>
+        <v>176.2166666666667</v>
       </c>
       <c r="D59" t="n">
-        <v>0.3476666666666666</v>
+        <v>0.3476666666666668</v>
       </c>
     </row>
     <row r="60">
@@ -1270,10 +1270,10 @@
         <v>1658</v>
       </c>
       <c r="C60" t="n">
-        <v>176.0333333333332</v>
+        <v>176.0333333333334</v>
       </c>
       <c r="D60" t="n">
-        <v>0.3473333333333333</v>
+        <v>0.3473333333333334</v>
       </c>
     </row>
     <row r="61">
@@ -1284,10 +1284,10 @@
         <v>1659</v>
       </c>
       <c r="C61" t="n">
-        <v>175.8499999999999</v>
+        <v>175.85</v>
       </c>
       <c r="D61" t="n">
-        <v>0.347</v>
+        <v>0.3470000000000001</v>
       </c>
     </row>
     <row r="62">
@@ -1298,10 +1298,10 @@
         <v>1660</v>
       </c>
       <c r="C62" t="n">
-        <v>175.6666666666666</v>
+        <v>175.6666666666667</v>
       </c>
       <c r="D62" t="n">
-        <v>0.3466666666666666</v>
+        <v>0.3466666666666668</v>
       </c>
     </row>
     <row r="63">
@@ -1312,10 +1312,10 @@
         <v>1661</v>
       </c>
       <c r="C63" t="n">
-        <v>175.4833333333332</v>
+        <v>175.4833333333333</v>
       </c>
       <c r="D63" t="n">
-        <v>0.3463333333333333</v>
+        <v>0.3463333333333334</v>
       </c>
     </row>
     <row r="64">
@@ -1326,10 +1326,10 @@
         <v>1662</v>
       </c>
       <c r="C64" t="n">
-        <v>175.2999999999999</v>
+        <v>175.3</v>
       </c>
       <c r="D64" t="n">
-        <v>0.346</v>
+        <v>0.3460000000000001</v>
       </c>
     </row>
     <row r="65">
@@ -1340,10 +1340,10 @@
         <v>1663</v>
       </c>
       <c r="C65" t="n">
-        <v>175.1166666666666</v>
+        <v>175.1166666666667</v>
       </c>
       <c r="D65" t="n">
-        <v>0.3456666666666666</v>
+        <v>0.3456666666666668</v>
       </c>
     </row>
     <row r="66">
@@ -1354,10 +1354,10 @@
         <v>1664</v>
       </c>
       <c r="C66" t="n">
-        <v>174.9333333333332</v>
+        <v>174.9333333333333</v>
       </c>
       <c r="D66" t="n">
-        <v>0.3453333333333333</v>
+        <v>0.3453333333333334</v>
       </c>
     </row>
     <row r="67">
@@ -1368,10 +1368,10 @@
         <v>1665</v>
       </c>
       <c r="C67" t="n">
-        <v>174.7499999999999</v>
+        <v>174.7500000000001</v>
       </c>
       <c r="D67" t="n">
-        <v>0.345</v>
+        <v>0.3450000000000001</v>
       </c>
     </row>
     <row r="68">
@@ -1382,10 +1382,10 @@
         <v>1666</v>
       </c>
       <c r="C68" t="n">
-        <v>174.5666666666666</v>
+        <v>174.5666666666667</v>
       </c>
       <c r="D68" t="n">
-        <v>0.3446666666666666</v>
+        <v>0.3446666666666668</v>
       </c>
     </row>
     <row r="69">
@@ -1396,10 +1396,10 @@
         <v>1667</v>
       </c>
       <c r="C69" t="n">
-        <v>174.3833333333333</v>
+        <v>174.3833333333334</v>
       </c>
       <c r="D69" t="n">
-        <v>0.3443333333333333</v>
+        <v>0.3443333333333334</v>
       </c>
     </row>
     <row r="70">
@@ -1410,10 +1410,10 @@
         <v>1668</v>
       </c>
       <c r="C70" t="n">
-        <v>174.1999999999999</v>
+        <v>174.2</v>
       </c>
       <c r="D70" t="n">
-        <v>0.344</v>
+        <v>0.3440000000000001</v>
       </c>
     </row>
     <row r="71">
@@ -1424,10 +1424,10 @@
         <v>1669</v>
       </c>
       <c r="C71" t="n">
-        <v>174.0166666666666</v>
+        <v>174.0166666666667</v>
       </c>
       <c r="D71" t="n">
-        <v>0.3436666666666666</v>
+        <v>0.3436666666666668</v>
       </c>
     </row>
     <row r="72">
@@ -1438,10 +1438,10 @@
         <v>1670</v>
       </c>
       <c r="C72" t="n">
-        <v>173.8333333333333</v>
+        <v>173.8333333333334</v>
       </c>
       <c r="D72" t="n">
-        <v>0.3433333333333333</v>
+        <v>0.3433333333333334</v>
       </c>
     </row>
     <row r="73">
@@ -1452,10 +1452,10 @@
         <v>1671</v>
       </c>
       <c r="C73" t="n">
-        <v>173.6499999999999</v>
+        <v>173.65</v>
       </c>
       <c r="D73" t="n">
-        <v>0.343</v>
+        <v>0.3430000000000001</v>
       </c>
     </row>
     <row r="74">
@@ -1466,10 +1466,10 @@
         <v>1672</v>
       </c>
       <c r="C74" t="n">
-        <v>173.4666666666666</v>
+        <v>173.4666666666667</v>
       </c>
       <c r="D74" t="n">
-        <v>0.3426666666666666</v>
+        <v>0.3426666666666668</v>
       </c>
     </row>
     <row r="75">
@@ -1480,10 +1480,10 @@
         <v>1673</v>
       </c>
       <c r="C75" t="n">
-        <v>173.2833333333332</v>
+        <v>173.2833333333334</v>
       </c>
       <c r="D75" t="n">
-        <v>0.3423333333333333</v>
+        <v>0.3423333333333334</v>
       </c>
     </row>
     <row r="76">
@@ -1494,10 +1494,10 @@
         <v>1674</v>
       </c>
       <c r="C76" t="n">
-        <v>173.0999999999999</v>
+        <v>173.1</v>
       </c>
       <c r="D76" t="n">
-        <v>0.342</v>
+        <v>0.3420000000000001</v>
       </c>
     </row>
     <row r="77">
@@ -1508,10 +1508,10 @@
         <v>1675</v>
       </c>
       <c r="C77" t="n">
-        <v>172.9166666666666</v>
+        <v>172.9166666666667</v>
       </c>
       <c r="D77" t="n">
-        <v>0.3416666666666666</v>
+        <v>0.3416666666666668</v>
       </c>
     </row>
     <row r="78">
@@ -1522,10 +1522,10 @@
         <v>1676</v>
       </c>
       <c r="C78" t="n">
-        <v>172.7333333333332</v>
+        <v>172.7333333333333</v>
       </c>
       <c r="D78" t="n">
-        <v>0.3413333333333333</v>
+        <v>0.3413333333333334</v>
       </c>
     </row>
     <row r="79">
@@ -1536,10 +1536,10 @@
         <v>1677</v>
       </c>
       <c r="C79" t="n">
-        <v>172.5499999999999</v>
+        <v>172.55</v>
       </c>
       <c r="D79" t="n">
-        <v>0.341</v>
+        <v>0.3410000000000001</v>
       </c>
     </row>
     <row r="80">
@@ -1550,10 +1550,10 @@
         <v>1678</v>
       </c>
       <c r="C80" t="n">
-        <v>172.3666666666666</v>
+        <v>172.3666666666667</v>
       </c>
       <c r="D80" t="n">
-        <v>0.3406666666666666</v>
+        <v>0.3406666666666668</v>
       </c>
     </row>
     <row r="81">
@@ -1564,10 +1564,10 @@
         <v>1679</v>
       </c>
       <c r="C81" t="n">
-        <v>172.1833333333333</v>
+        <v>172.1833333333334</v>
       </c>
       <c r="D81" t="n">
-        <v>0.3403333333333333</v>
+        <v>0.3403333333333334</v>
       </c>
     </row>
     <row r="82">
@@ -1578,10 +1578,10 @@
         <v>1680</v>
       </c>
       <c r="C82" t="n">
-        <v>171.9999999999999</v>
+        <v>172.0000000000001</v>
       </c>
       <c r="D82" t="n">
-        <v>0.34</v>
+        <v>0.3400000000000001</v>
       </c>
     </row>
     <row r="83">
@@ -1592,10 +1592,10 @@
         <v>1681</v>
       </c>
       <c r="C83" t="n">
-        <v>171.8166666666666</v>
+        <v>171.8166666666667</v>
       </c>
       <c r="D83" t="n">
-        <v>0.3396666666666666</v>
+        <v>0.3396666666666668</v>
       </c>
     </row>
     <row r="84">
@@ -1606,10 +1606,10 @@
         <v>1682</v>
       </c>
       <c r="C84" t="n">
-        <v>171.6333333333333</v>
+        <v>171.6333333333334</v>
       </c>
       <c r="D84" t="n">
-        <v>0.3393333333333333</v>
+        <v>0.3393333333333334</v>
       </c>
     </row>
     <row r="85">
@@ -1620,10 +1620,10 @@
         <v>1683</v>
       </c>
       <c r="C85" t="n">
-        <v>171.4499999999999</v>
+        <v>171.45</v>
       </c>
       <c r="D85" t="n">
-        <v>0.339</v>
+        <v>0.3390000000000001</v>
       </c>
     </row>
     <row r="86">
@@ -1634,10 +1634,10 @@
         <v>1684</v>
       </c>
       <c r="C86" t="n">
-        <v>171.2666666666666</v>
+        <v>171.2666666666667</v>
       </c>
       <c r="D86" t="n">
-        <v>0.3386666666666666</v>
+        <v>0.3386666666666668</v>
       </c>
     </row>
     <row r="87">
@@ -1648,10 +1648,10 @@
         <v>1685</v>
       </c>
       <c r="C87" t="n">
-        <v>171.0833333333333</v>
+        <v>171.0833333333334</v>
       </c>
       <c r="D87" t="n">
-        <v>0.3383333333333333</v>
+        <v>0.3383333333333334</v>
       </c>
     </row>
     <row r="88">
@@ -1662,10 +1662,10 @@
         <v>1686</v>
       </c>
       <c r="C88" t="n">
-        <v>170.8999999999999</v>
+        <v>170.9</v>
       </c>
       <c r="D88" t="n">
-        <v>0.338</v>
+        <v>0.3380000000000001</v>
       </c>
     </row>
     <row r="89">
@@ -1676,10 +1676,10 @@
         <v>1687</v>
       </c>
       <c r="C89" t="n">
-        <v>170.7166666666666</v>
+        <v>170.7166666666667</v>
       </c>
       <c r="D89" t="n">
-        <v>0.3376666666666666</v>
+        <v>0.3376666666666668</v>
       </c>
     </row>
     <row r="90">
@@ -1690,10 +1690,10 @@
         <v>1688</v>
       </c>
       <c r="C90" t="n">
-        <v>170.5333333333332</v>
+        <v>170.5333333333334</v>
       </c>
       <c r="D90" t="n">
-        <v>0.3373333333333333</v>
+        <v>0.3373333333333334</v>
       </c>
     </row>
     <row r="91">
@@ -1704,10 +1704,10 @@
         <v>1689</v>
       </c>
       <c r="C91" t="n">
-        <v>170.3499999999999</v>
+        <v>170.35</v>
       </c>
       <c r="D91" t="n">
-        <v>0.337</v>
+        <v>0.3370000000000001</v>
       </c>
     </row>
     <row r="92">
@@ -1718,10 +1718,10 @@
         <v>1690</v>
       </c>
       <c r="C92" t="n">
-        <v>170.1666666666666</v>
+        <v>170.1666666666667</v>
       </c>
       <c r="D92" t="n">
-        <v>0.3366666666666666</v>
+        <v>0.3366666666666668</v>
       </c>
     </row>
     <row r="93">
@@ -1732,10 +1732,10 @@
         <v>1691</v>
       </c>
       <c r="C93" t="n">
-        <v>169.9833333333332</v>
+        <v>169.9833333333333</v>
       </c>
       <c r="D93" t="n">
-        <v>0.3363333333333333</v>
+        <v>0.3363333333333334</v>
       </c>
     </row>
     <row r="94">
@@ -1746,10 +1746,10 @@
         <v>1692</v>
       </c>
       <c r="C94" t="n">
-        <v>169.7999999999999</v>
+        <v>169.8</v>
       </c>
       <c r="D94" t="n">
-        <v>0.336</v>
+        <v>0.3360000000000001</v>
       </c>
     </row>
     <row r="95">
@@ -1760,10 +1760,10 @@
         <v>1693</v>
       </c>
       <c r="C95" t="n">
-        <v>169.6166666666666</v>
+        <v>169.6166666666667</v>
       </c>
       <c r="D95" t="n">
-        <v>0.3356666666666666</v>
+        <v>0.3356666666666668</v>
       </c>
     </row>
     <row r="96">
@@ -1774,10 +1774,10 @@
         <v>1694</v>
       </c>
       <c r="C96" t="n">
-        <v>169.4333333333333</v>
+        <v>169.4333333333334</v>
       </c>
       <c r="D96" t="n">
-        <v>0.3353333333333333</v>
+        <v>0.3353333333333335</v>
       </c>
     </row>
     <row r="97">
@@ -1788,10 +1788,10 @@
         <v>1695</v>
       </c>
       <c r="C97" t="n">
-        <v>169.2499999999999</v>
+        <v>169.2500000000001</v>
       </c>
       <c r="D97" t="n">
-        <v>0.335</v>
+        <v>0.3350000000000001</v>
       </c>
     </row>
     <row r="98">
@@ -1802,10 +1802,10 @@
         <v>1696</v>
       </c>
       <c r="C98" t="n">
-        <v>169.0666666666666</v>
+        <v>169.0666666666667</v>
       </c>
       <c r="D98" t="n">
-        <v>0.3346666666666667</v>
+        <v>0.3346666666666668</v>
       </c>
     </row>
     <row r="99">
@@ -1816,10 +1816,10 @@
         <v>1697</v>
       </c>
       <c r="C99" t="n">
-        <v>168.8833333333333</v>
+        <v>168.8833333333334</v>
       </c>
       <c r="D99" t="n">
-        <v>0.3343333333333333</v>
+        <v>0.3343333333333335</v>
       </c>
     </row>
     <row r="100">
@@ -1830,10 +1830,10 @@
         <v>1698</v>
       </c>
       <c r="C100" t="n">
-        <v>168.6999999999999</v>
+        <v>168.7</v>
       </c>
       <c r="D100" t="n">
-        <v>0.334</v>
+        <v>0.3340000000000001</v>
       </c>
     </row>
     <row r="101">
@@ -1844,10 +1844,10 @@
         <v>1699</v>
       </c>
       <c r="C101" t="n">
-        <v>168.5166666666666</v>
+        <v>168.5166666666667</v>
       </c>
       <c r="D101" t="n">
-        <v>0.3336666666666667</v>
+        <v>0.3336666666666668</v>
       </c>
     </row>
     <row r="102">
@@ -1858,10 +1858,10 @@
         <v>1700</v>
       </c>
       <c r="C102" t="n">
-        <v>168.3333333333333</v>
+        <v>168.3333333333334</v>
       </c>
       <c r="D102" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.3333333333333335</v>
       </c>
     </row>
     <row r="103">
@@ -1872,10 +1872,10 @@
         <v>1701</v>
       </c>
       <c r="C103" t="n">
-        <v>168.1499999999999</v>
+        <v>168.15</v>
       </c>
       <c r="D103" t="n">
-        <v>0.333</v>
+        <v>0.3330000000000001</v>
       </c>
     </row>
     <row r="104">
@@ -1886,10 +1886,10 @@
         <v>1702</v>
       </c>
       <c r="C104" t="n">
-        <v>167.9666666666666</v>
+        <v>167.9666666666667</v>
       </c>
       <c r="D104" t="n">
-        <v>0.3326666666666667</v>
+        <v>0.3326666666666668</v>
       </c>
     </row>
     <row r="105">
@@ -1900,10 +1900,10 @@
         <v>1703</v>
       </c>
       <c r="C105" t="n">
-        <v>167.7833333333332</v>
+        <v>167.7833333333334</v>
       </c>
       <c r="D105" t="n">
-        <v>0.3323333333333333</v>
+        <v>0.3323333333333335</v>
       </c>
     </row>
     <row r="106">
@@ -1914,10 +1914,10 @@
         <v>1704</v>
       </c>
       <c r="C106" t="n">
-        <v>167.5999999999999</v>
+        <v>167.6</v>
       </c>
       <c r="D106" t="n">
-        <v>0.332</v>
+        <v>0.3320000000000001</v>
       </c>
     </row>
     <row r="107">
@@ -1928,10 +1928,10 @@
         <v>1705</v>
       </c>
       <c r="C107" t="n">
-        <v>167.4166666666666</v>
+        <v>167.4166666666667</v>
       </c>
       <c r="D107" t="n">
-        <v>0.3316666666666667</v>
+        <v>0.3316666666666668</v>
       </c>
     </row>
     <row r="108">
@@ -1942,10 +1942,10 @@
         <v>1706</v>
       </c>
       <c r="C108" t="n">
-        <v>167.2333333333332</v>
+        <v>167.2333333333333</v>
       </c>
       <c r="D108" t="n">
-        <v>0.3313333333333333</v>
+        <v>0.3313333333333335</v>
       </c>
     </row>
     <row r="109">
@@ -1956,10 +1956,10 @@
         <v>1707</v>
       </c>
       <c r="C109" t="n">
-        <v>167.05</v>
+        <v>167.0500000000001</v>
       </c>
       <c r="D109" t="n">
-        <v>0.331</v>
+        <v>0.3310000000000001</v>
       </c>
     </row>
     <row r="110">
@@ -1970,10 +1970,10 @@
         <v>1708</v>
       </c>
       <c r="C110" t="n">
-        <v>166.8666666666666</v>
+        <v>166.8666666666667</v>
       </c>
       <c r="D110" t="n">
-        <v>0.3306666666666667</v>
+        <v>0.3306666666666668</v>
       </c>
     </row>
     <row r="111">
@@ -1984,10 +1984,10 @@
         <v>1709</v>
       </c>
       <c r="C111" t="n">
-        <v>166.6833333333333</v>
+        <v>166.6833333333334</v>
       </c>
       <c r="D111" t="n">
-        <v>0.3303333333333333</v>
+        <v>0.3303333333333335</v>
       </c>
     </row>
     <row r="112">
@@ -1998,10 +1998,10 @@
         <v>1710</v>
       </c>
       <c r="C112" t="n">
-        <v>166.4999999999999</v>
+        <v>166.5000000000001</v>
       </c>
       <c r="D112" t="n">
-        <v>0.33</v>
+        <v>0.3300000000000001</v>
       </c>
     </row>
     <row r="113">
@@ -2012,10 +2012,10 @@
         <v>1711</v>
       </c>
       <c r="C113" t="n">
-        <v>166.3166666666666</v>
+        <v>166.3166666666667</v>
       </c>
       <c r="D113" t="n">
-        <v>0.3296666666666667</v>
+        <v>0.3296666666666668</v>
       </c>
     </row>
     <row r="114">
@@ -2026,10 +2026,10 @@
         <v>1712</v>
       </c>
       <c r="C114" t="n">
-        <v>166.1333333333333</v>
+        <v>166.1333333333334</v>
       </c>
       <c r="D114" t="n">
-        <v>0.3293333333333333</v>
+        <v>0.3293333333333335</v>
       </c>
     </row>
     <row r="115">
@@ -2040,10 +2040,10 @@
         <v>1713</v>
       </c>
       <c r="C115" t="n">
-        <v>165.9499999999999</v>
+        <v>165.95</v>
       </c>
       <c r="D115" t="n">
-        <v>0.329</v>
+        <v>0.3290000000000001</v>
       </c>
     </row>
     <row r="116">
@@ -2054,10 +2054,10 @@
         <v>1714</v>
       </c>
       <c r="C116" t="n">
-        <v>165.7666666666666</v>
+        <v>165.7666666666667</v>
       </c>
       <c r="D116" t="n">
-        <v>0.3286666666666667</v>
+        <v>0.3286666666666668</v>
       </c>
     </row>
     <row r="117">
@@ -2068,10 +2068,10 @@
         <v>1715</v>
       </c>
       <c r="C117" t="n">
-        <v>165.5833333333333</v>
+        <v>165.5833333333334</v>
       </c>
       <c r="D117" t="n">
-        <v>0.3283333333333333</v>
+        <v>0.3283333333333335</v>
       </c>
     </row>
     <row r="118">
@@ -2082,10 +2082,10 @@
         <v>1716</v>
       </c>
       <c r="C118" t="n">
-        <v>165.3999999999999</v>
+        <v>165.4</v>
       </c>
       <c r="D118" t="n">
-        <v>0.328</v>
+        <v>0.3280000000000001</v>
       </c>
     </row>
     <row r="119">
@@ -2096,10 +2096,10 @@
         <v>1717</v>
       </c>
       <c r="C119" t="n">
-        <v>165.2166666666666</v>
+        <v>165.2166666666667</v>
       </c>
       <c r="D119" t="n">
-        <v>0.3276666666666667</v>
+        <v>0.3276666666666668</v>
       </c>
     </row>
     <row r="120">
@@ -2110,10 +2110,10 @@
         <v>1718</v>
       </c>
       <c r="C120" t="n">
-        <v>165.0333333333332</v>
+        <v>165.0333333333334</v>
       </c>
       <c r="D120" t="n">
-        <v>0.3273333333333333</v>
+        <v>0.3273333333333335</v>
       </c>
     </row>
     <row r="121">
@@ -2124,10 +2124,10 @@
         <v>1719</v>
       </c>
       <c r="C121" t="n">
-        <v>164.8499999999999</v>
+        <v>164.85</v>
       </c>
       <c r="D121" t="n">
-        <v>0.327</v>
+        <v>0.3270000000000001</v>
       </c>
     </row>
     <row r="122">
@@ -2138,10 +2138,10 @@
         <v>1720</v>
       </c>
       <c r="C122" t="n">
-        <v>164.6666666666666</v>
+        <v>164.6666666666667</v>
       </c>
       <c r="D122" t="n">
-        <v>0.3266666666666667</v>
+        <v>0.3266666666666668</v>
       </c>
     </row>
     <row r="123">
@@ -2152,10 +2152,10 @@
         <v>1721</v>
       </c>
       <c r="C123" t="n">
-        <v>164.4833333333333</v>
+        <v>164.4833333333334</v>
       </c>
       <c r="D123" t="n">
-        <v>0.3263333333333333</v>
+        <v>0.3263333333333335</v>
       </c>
     </row>
     <row r="124">
@@ -2166,10 +2166,10 @@
         <v>1722</v>
       </c>
       <c r="C124" t="n">
-        <v>164.3</v>
+        <v>164.3000000000001</v>
       </c>
       <c r="D124" t="n">
-        <v>0.326</v>
+        <v>0.3260000000000001</v>
       </c>
     </row>
     <row r="125">
@@ -2180,10 +2180,10 @@
         <v>1723</v>
       </c>
       <c r="C125" t="n">
-        <v>164.1166666666666</v>
+        <v>164.1166666666667</v>
       </c>
       <c r="D125" t="n">
-        <v>0.3256666666666667</v>
+        <v>0.3256666666666668</v>
       </c>
     </row>
     <row r="126">
@@ -2194,10 +2194,10 @@
         <v>1724</v>
       </c>
       <c r="C126" t="n">
-        <v>163.9333333333333</v>
+        <v>163.9333333333334</v>
       </c>
       <c r="D126" t="n">
-        <v>0.3253333333333333</v>
+        <v>0.3253333333333335</v>
       </c>
     </row>
     <row r="127">
@@ -2208,10 +2208,10 @@
         <v>1725</v>
       </c>
       <c r="C127" t="n">
-        <v>163.7499999999999</v>
+        <v>163.7500000000001</v>
       </c>
       <c r="D127" t="n">
-        <v>0.325</v>
+        <v>0.3250000000000001</v>
       </c>
     </row>
     <row r="128">
@@ -2222,10 +2222,10 @@
         <v>1726</v>
       </c>
       <c r="C128" t="n">
-        <v>163.5666666666666</v>
+        <v>163.5666666666667</v>
       </c>
       <c r="D128" t="n">
-        <v>0.3246666666666667</v>
+        <v>0.3246666666666668</v>
       </c>
     </row>
     <row r="129">
@@ -2236,10 +2236,10 @@
         <v>1727</v>
       </c>
       <c r="C129" t="n">
-        <v>163.3833333333333</v>
+        <v>163.3833333333334</v>
       </c>
       <c r="D129" t="n">
-        <v>0.3243333333333333</v>
+        <v>0.3243333333333335</v>
       </c>
     </row>
     <row r="130">
@@ -2250,10 +2250,10 @@
         <v>1728</v>
       </c>
       <c r="C130" t="n">
-        <v>163.1999999999999</v>
+        <v>163.2</v>
       </c>
       <c r="D130" t="n">
-        <v>0.324</v>
+        <v>0.3240000000000001</v>
       </c>
     </row>
     <row r="131">
@@ -2264,10 +2264,10 @@
         <v>1729</v>
       </c>
       <c r="C131" t="n">
-        <v>163.0166666666666</v>
+        <v>163.0166666666667</v>
       </c>
       <c r="D131" t="n">
-        <v>0.3236666666666667</v>
+        <v>0.3236666666666668</v>
       </c>
     </row>
     <row r="132">
@@ -2278,10 +2278,10 @@
         <v>1730</v>
       </c>
       <c r="C132" t="n">
-        <v>162.8333333333333</v>
+        <v>162.8333333333334</v>
       </c>
       <c r="D132" t="n">
-        <v>0.3233333333333333</v>
+        <v>0.3233333333333335</v>
       </c>
     </row>
     <row r="133">
@@ -2292,10 +2292,10 @@
         <v>1731</v>
       </c>
       <c r="C133" t="n">
-        <v>162.6499999999999</v>
+        <v>162.65</v>
       </c>
       <c r="D133" t="n">
-        <v>0.323</v>
+        <v>0.3230000000000001</v>
       </c>
     </row>
     <row r="134">
@@ -2306,10 +2306,10 @@
         <v>1732</v>
       </c>
       <c r="C134" t="n">
-        <v>162.4666666666666</v>
+        <v>162.4666666666667</v>
       </c>
       <c r="D134" t="n">
-        <v>0.3226666666666667</v>
+        <v>0.3226666666666668</v>
       </c>
     </row>
     <row r="135">
@@ -2320,10 +2320,10 @@
         <v>1733</v>
       </c>
       <c r="C135" t="n">
-        <v>162.2833333333332</v>
+        <v>162.2833333333334</v>
       </c>
       <c r="D135" t="n">
-        <v>0.3223333333333332</v>
+        <v>0.3223333333333335</v>
       </c>
     </row>
     <row r="136">
@@ -2334,10 +2334,10 @@
         <v>1734</v>
       </c>
       <c r="C136" t="n">
-        <v>162.0999999999999</v>
+        <v>162.1</v>
       </c>
       <c r="D136" t="n">
-        <v>0.322</v>
+        <v>0.3220000000000001</v>
       </c>
     </row>
     <row r="137">
@@ -2348,10 +2348,10 @@
         <v>1735</v>
       </c>
       <c r="C137" t="n">
-        <v>161.9166666666666</v>
+        <v>161.9166666666667</v>
       </c>
       <c r="D137" t="n">
-        <v>0.3216666666666667</v>
+        <v>0.3216666666666668</v>
       </c>
     </row>
     <row r="138">
@@ -2362,10 +2362,10 @@
         <v>1736</v>
       </c>
       <c r="C138" t="n">
-        <v>161.7333333333333</v>
+        <v>161.7333333333334</v>
       </c>
       <c r="D138" t="n">
-        <v>0.3213333333333332</v>
+        <v>0.3213333333333335</v>
       </c>
     </row>
     <row r="139">
@@ -2376,10 +2376,10 @@
         <v>1737</v>
       </c>
       <c r="C139" t="n">
-        <v>161.55</v>
+        <v>161.5500000000001</v>
       </c>
       <c r="D139" t="n">
-        <v>0.321</v>
+        <v>0.3210000000000001</v>
       </c>
     </row>
     <row r="140">
@@ -2390,10 +2390,10 @@
         <v>1738</v>
       </c>
       <c r="C140" t="n">
-        <v>161.3666666666666</v>
+        <v>161.3666666666667</v>
       </c>
       <c r="D140" t="n">
-        <v>0.3206666666666667</v>
+        <v>0.3206666666666668</v>
       </c>
     </row>
     <row r="141">
@@ -2404,10 +2404,10 @@
         <v>1739</v>
       </c>
       <c r="C141" t="n">
-        <v>161.1833333333333</v>
+        <v>161.1833333333334</v>
       </c>
       <c r="D141" t="n">
-        <v>0.3203333333333332</v>
+        <v>0.3203333333333335</v>
       </c>
     </row>
     <row r="142">
@@ -2418,10 +2418,10 @@
         <v>1740</v>
       </c>
       <c r="C142" t="n">
-        <v>160.9999999999999</v>
+        <v>161.0000000000001</v>
       </c>
       <c r="D142" t="n">
-        <v>0.32</v>
+        <v>0.3200000000000001</v>
       </c>
     </row>
     <row r="143">
@@ -2432,10 +2432,10 @@
         <v>1741</v>
       </c>
       <c r="C143" t="n">
-        <v>160.8166666666666</v>
+        <v>160.8166666666667</v>
       </c>
       <c r="D143" t="n">
-        <v>0.3196666666666667</v>
+        <v>0.3196666666666668</v>
       </c>
     </row>
     <row r="144">
@@ -2446,10 +2446,10 @@
         <v>1742</v>
       </c>
       <c r="C144" t="n">
-        <v>160.6333333333333</v>
+        <v>160.6333333333334</v>
       </c>
       <c r="D144" t="n">
-        <v>0.3193333333333332</v>
+        <v>0.3193333333333335</v>
       </c>
     </row>
     <row r="145">
@@ -2460,10 +2460,10 @@
         <v>1743</v>
       </c>
       <c r="C145" t="n">
-        <v>160.4499999999999</v>
+        <v>160.45</v>
       </c>
       <c r="D145" t="n">
-        <v>0.319</v>
+        <v>0.3190000000000001</v>
       </c>
     </row>
     <row r="146">
@@ -2474,10 +2474,10 @@
         <v>1744</v>
       </c>
       <c r="C146" t="n">
-        <v>160.2666666666666</v>
+        <v>160.2666666666667</v>
       </c>
       <c r="D146" t="n">
-        <v>0.3186666666666667</v>
+        <v>0.3186666666666668</v>
       </c>
     </row>
     <row r="147">
@@ -2488,10 +2488,10 @@
         <v>1745</v>
       </c>
       <c r="C147" t="n">
-        <v>160.0833333333333</v>
+        <v>160.0833333333334</v>
       </c>
       <c r="D147" t="n">
-        <v>0.3183333333333332</v>
+        <v>0.3183333333333335</v>
       </c>
     </row>
     <row r="148">
@@ -2502,10 +2502,10 @@
         <v>1746</v>
       </c>
       <c r="C148" t="n">
-        <v>159.8999999999999</v>
+        <v>159.9</v>
       </c>
       <c r="D148" t="n">
-        <v>0.3179999999999999</v>
+        <v>0.3180000000000001</v>
       </c>
     </row>
     <row r="149">
@@ -2516,10 +2516,10 @@
         <v>1747</v>
       </c>
       <c r="C149" t="n">
-        <v>159.7166666666666</v>
+        <v>159.7166666666667</v>
       </c>
       <c r="D149" t="n">
-        <v>0.3176666666666667</v>
+        <v>0.3176666666666668</v>
       </c>
     </row>
     <row r="150">
@@ -2530,10 +2530,10 @@
         <v>1748</v>
       </c>
       <c r="C150" t="n">
-        <v>159.5333333333332</v>
+        <v>159.5333333333334</v>
       </c>
       <c r="D150" t="n">
-        <v>0.3173333333333332</v>
+        <v>0.3173333333333335</v>
       </c>
     </row>
     <row r="151">
@@ -2544,10 +2544,10 @@
         <v>1749</v>
       </c>
       <c r="C151" t="n">
-        <v>159.35</v>
+        <v>159.3500000000001</v>
       </c>
       <c r="D151" t="n">
-        <v>0.3169999999999999</v>
+        <v>0.3170000000000001</v>
       </c>
     </row>
     <row r="152">
@@ -2558,10 +2558,10 @@
         <v>1750</v>
       </c>
       <c r="C152" t="n">
-        <v>159.1666666666666</v>
+        <v>159.1666666666667</v>
       </c>
       <c r="D152" t="n">
-        <v>0.3166666666666667</v>
+        <v>0.3166666666666668</v>
       </c>
     </row>
     <row r="153">
@@ -2572,10 +2572,10 @@
         <v>1751</v>
       </c>
       <c r="C153" t="n">
-        <v>158.9833333333333</v>
+        <v>158.9833333333334</v>
       </c>
       <c r="D153" t="n">
-        <v>0.3163333333333332</v>
+        <v>0.3163333333333335</v>
       </c>
     </row>
     <row r="154">
@@ -2586,10 +2586,10 @@
         <v>1752</v>
       </c>
       <c r="C154" t="n">
-        <v>158.8</v>
+        <v>158.8000000000001</v>
       </c>
       <c r="D154" t="n">
-        <v>0.3159999999999999</v>
+        <v>0.3160000000000001</v>
       </c>
     </row>
     <row r="155">
@@ -2600,10 +2600,10 @@
         <v>1753</v>
       </c>
       <c r="C155" t="n">
-        <v>158.6166666666666</v>
+        <v>158.6166666666667</v>
       </c>
       <c r="D155" t="n">
-        <v>0.3156666666666667</v>
+        <v>0.3156666666666668</v>
       </c>
     </row>
     <row r="156">
@@ -2614,10 +2614,10 @@
         <v>1754</v>
       </c>
       <c r="C156" t="n">
-        <v>158.4333333333333</v>
+        <v>158.4333333333334</v>
       </c>
       <c r="D156" t="n">
-        <v>0.3153333333333332</v>
+        <v>0.3153333333333335</v>
       </c>
     </row>
     <row r="157">
@@ -2628,10 +2628,10 @@
         <v>1755</v>
       </c>
       <c r="C157" t="n">
-        <v>158.2499999999999</v>
+        <v>158.2500000000001</v>
       </c>
       <c r="D157" t="n">
-        <v>0.3149999999999999</v>
+        <v>0.3150000000000001</v>
       </c>
     </row>
     <row r="158">
@@ -2642,10 +2642,10 @@
         <v>1756</v>
       </c>
       <c r="C158" t="n">
-        <v>158.0666666666666</v>
+        <v>158.0666666666667</v>
       </c>
       <c r="D158" t="n">
-        <v>0.3146666666666667</v>
+        <v>0.3146666666666668</v>
       </c>
     </row>
     <row r="159">
@@ -2656,10 +2656,10 @@
         <v>1757</v>
       </c>
       <c r="C159" t="n">
-        <v>157.8833333333333</v>
+        <v>157.8833333333334</v>
       </c>
       <c r="D159" t="n">
-        <v>0.3143333333333332</v>
+        <v>0.3143333333333335</v>
       </c>
     </row>
     <row r="160">
@@ -2670,10 +2670,10 @@
         <v>1758</v>
       </c>
       <c r="C160" t="n">
-        <v>157.6999999999999</v>
+        <v>157.7</v>
       </c>
       <c r="D160" t="n">
-        <v>0.3139999999999999</v>
+        <v>0.3140000000000001</v>
       </c>
     </row>
     <row r="161">
@@ -2684,10 +2684,10 @@
         <v>1759</v>
       </c>
       <c r="C161" t="n">
-        <v>157.5166666666666</v>
+        <v>157.5166666666667</v>
       </c>
       <c r="D161" t="n">
-        <v>0.3136666666666666</v>
+        <v>0.3136666666666668</v>
       </c>
     </row>
     <row r="162">
@@ -2698,10 +2698,10 @@
         <v>1760</v>
       </c>
       <c r="C162" t="n">
-        <v>157.3333333333333</v>
+        <v>157.3333333333334</v>
       </c>
       <c r="D162" t="n">
-        <v>0.3133333333333332</v>
+        <v>0.3133333333333335</v>
       </c>
     </row>
     <row r="163">
@@ -2712,10 +2712,10 @@
         <v>1761</v>
       </c>
       <c r="C163" t="n">
-        <v>157.1499999999999</v>
+        <v>157.15</v>
       </c>
       <c r="D163" t="n">
-        <v>0.3129999999999999</v>
+        <v>0.3130000000000001</v>
       </c>
     </row>
     <row r="164">
@@ -2726,10 +2726,10 @@
         <v>1762</v>
       </c>
       <c r="C164" t="n">
-        <v>156.9666666666666</v>
+        <v>156.9666666666667</v>
       </c>
       <c r="D164" t="n">
-        <v>0.3126666666666666</v>
+        <v>0.3126666666666668</v>
       </c>
     </row>
     <row r="165">
@@ -2740,10 +2740,10 @@
         <v>1763</v>
       </c>
       <c r="C165" t="n">
-        <v>156.7833333333333</v>
+        <v>156.7833333333334</v>
       </c>
       <c r="D165" t="n">
-        <v>0.3123333333333334</v>
+        <v>0.3123333333333335</v>
       </c>
     </row>
     <row r="166">
@@ -2754,10 +2754,10 @@
         <v>1764</v>
       </c>
       <c r="C166" t="n">
-        <v>156.6</v>
+        <v>156.6000000000001</v>
       </c>
       <c r="D166" t="n">
-        <v>0.3119999999999999</v>
+        <v>0.3120000000000001</v>
       </c>
     </row>
     <row r="167">
@@ -2768,10 +2768,10 @@
         <v>1765</v>
       </c>
       <c r="C167" t="n">
-        <v>156.4166666666666</v>
+        <v>156.4166666666667</v>
       </c>
       <c r="D167" t="n">
-        <v>0.3116666666666666</v>
+        <v>0.3116666666666668</v>
       </c>
     </row>
     <row r="168">
@@ -2782,10 +2782,10 @@
         <v>1766</v>
       </c>
       <c r="C168" t="n">
-        <v>156.2333333333333</v>
+        <v>156.2333333333334</v>
       </c>
       <c r="D168" t="n">
-        <v>0.3113333333333334</v>
+        <v>0.3113333333333335</v>
       </c>
     </row>
     <row r="169">
@@ -2796,10 +2796,10 @@
         <v>1767</v>
       </c>
       <c r="C169" t="n">
-        <v>156.05</v>
+        <v>156.0500000000001</v>
       </c>
       <c r="D169" t="n">
-        <v>0.3109999999999999</v>
+        <v>0.3110000000000001</v>
       </c>
     </row>
     <row r="170">
@@ -2810,10 +2810,10 @@
         <v>1768</v>
       </c>
       <c r="C170" t="n">
-        <v>155.8666666666666</v>
+        <v>155.8666666666667</v>
       </c>
       <c r="D170" t="n">
-        <v>0.3106666666666666</v>
+        <v>0.3106666666666668</v>
       </c>
     </row>
     <row r="171">
@@ -2824,10 +2824,10 @@
         <v>1769</v>
       </c>
       <c r="C171" t="n">
-        <v>155.6833333333333</v>
+        <v>155.6833333333334</v>
       </c>
       <c r="D171" t="n">
-        <v>0.3103333333333333</v>
+        <v>0.3103333333333335</v>
       </c>
     </row>
     <row r="172">
@@ -2838,10 +2838,10 @@
         <v>1770</v>
       </c>
       <c r="C172" t="n">
-        <v>155.4999999999999</v>
+        <v>155.5000000000001</v>
       </c>
       <c r="D172" t="n">
-        <v>0.3099999999999999</v>
+        <v>0.3100000000000001</v>
       </c>
     </row>
     <row r="173">
@@ -2852,10 +2852,10 @@
         <v>1771</v>
       </c>
       <c r="C173" t="n">
-        <v>155.3166666666666</v>
+        <v>155.3166666666667</v>
       </c>
       <c r="D173" t="n">
-        <v>0.3096666666666666</v>
+        <v>0.3096666666666668</v>
       </c>
     </row>
     <row r="174">
@@ -2866,10 +2866,10 @@
         <v>1772</v>
       </c>
       <c r="C174" t="n">
-        <v>155.1333333333333</v>
+        <v>155.1333333333334</v>
       </c>
       <c r="D174" t="n">
-        <v>0.3093333333333333</v>
+        <v>0.3093333333333335</v>
       </c>
     </row>
     <row r="175">
@@ -2880,10 +2880,10 @@
         <v>1773</v>
       </c>
       <c r="C175" t="n">
-        <v>154.9499999999999</v>
+        <v>154.95</v>
       </c>
       <c r="D175" t="n">
-        <v>0.3089999999999999</v>
+        <v>0.3090000000000002</v>
       </c>
     </row>
     <row r="176">
@@ -2894,10 +2894,10 @@
         <v>1774</v>
       </c>
       <c r="C176" t="n">
-        <v>154.7666666666666</v>
+        <v>154.7666666666667</v>
       </c>
       <c r="D176" t="n">
-        <v>0.3086666666666666</v>
+        <v>0.3086666666666668</v>
       </c>
     </row>
     <row r="177">
@@ -2908,10 +2908,10 @@
         <v>1775</v>
       </c>
       <c r="C177" t="n">
-        <v>154.5833333333333</v>
+        <v>154.5833333333334</v>
       </c>
       <c r="D177" t="n">
-        <v>0.3083333333333333</v>
+        <v>0.3083333333333335</v>
       </c>
     </row>
     <row r="178">
@@ -2922,10 +2922,10 @@
         <v>1776</v>
       </c>
       <c r="C178" t="n">
-        <v>154.3999999999999</v>
+        <v>154.4</v>
       </c>
       <c r="D178" t="n">
-        <v>0.3079999999999999</v>
+        <v>0.3080000000000002</v>
       </c>
     </row>
     <row r="179">
@@ -2936,10 +2936,10 @@
         <v>1777</v>
       </c>
       <c r="C179" t="n">
-        <v>154.2166666666666</v>
+        <v>154.2166666666668</v>
       </c>
       <c r="D179" t="n">
-        <v>0.3076666666666666</v>
+        <v>0.3076666666666668</v>
       </c>
     </row>
     <row r="180">
@@ -2950,10 +2950,10 @@
         <v>1778</v>
       </c>
       <c r="C180" t="n">
-        <v>154.0333333333333</v>
+        <v>154.0333333333334</v>
       </c>
       <c r="D180" t="n">
-        <v>0.3073333333333333</v>
+        <v>0.3073333333333335</v>
       </c>
     </row>
     <row r="181">
@@ -2964,10 +2964,10 @@
         <v>1779</v>
       </c>
       <c r="C181" t="n">
-        <v>153.85</v>
+        <v>153.8500000000001</v>
       </c>
       <c r="D181" t="n">
-        <v>0.3069999999999999</v>
+        <v>0.3070000000000002</v>
       </c>
     </row>
     <row r="182">
@@ -2978,10 +2978,10 @@
         <v>1780</v>
       </c>
       <c r="C182" t="n">
-        <v>153.6666666666666</v>
+        <v>153.6666666666667</v>
       </c>
       <c r="D182" t="n">
-        <v>0.3066666666666666</v>
+        <v>0.3066666666666668</v>
       </c>
     </row>
     <row r="183">
@@ -2992,10 +2992,10 @@
         <v>1781</v>
       </c>
       <c r="C183" t="n">
-        <v>153.4833333333333</v>
+        <v>153.4833333333334</v>
       </c>
       <c r="D183" t="n">
-        <v>0.3063333333333333</v>
+        <v>0.3063333333333335</v>
       </c>
     </row>
     <row r="184">
@@ -3006,10 +3006,10 @@
         <v>1782</v>
       </c>
       <c r="C184" t="n">
-        <v>153.3</v>
+        <v>153.3000000000001</v>
       </c>
       <c r="D184" t="n">
-        <v>0.3059999999999999</v>
+        <v>0.3060000000000002</v>
       </c>
     </row>
     <row r="185">
@@ -3020,10 +3020,10 @@
         <v>1783</v>
       </c>
       <c r="C185" t="n">
-        <v>153.1166666666666</v>
+        <v>153.1166666666667</v>
       </c>
       <c r="D185" t="n">
-        <v>0.3056666666666666</v>
+        <v>0.3056666666666668</v>
       </c>
     </row>
     <row r="186">
@@ -3034,10 +3034,10 @@
         <v>1784</v>
       </c>
       <c r="C186" t="n">
-        <v>152.9333333333333</v>
+        <v>152.9333333333334</v>
       </c>
       <c r="D186" t="n">
-        <v>0.3053333333333333</v>
+        <v>0.3053333333333335</v>
       </c>
     </row>
     <row r="187">
@@ -3048,10 +3048,10 @@
         <v>1785</v>
       </c>
       <c r="C187" t="n">
-        <v>152.7499999999999</v>
+        <v>152.7500000000001</v>
       </c>
       <c r="D187" t="n">
-        <v>0.3049999999999999</v>
+        <v>0.3050000000000002</v>
       </c>
     </row>
     <row r="188">
@@ -3062,10 +3062,10 @@
         <v>1786</v>
       </c>
       <c r="C188" t="n">
-        <v>152.5666666666666</v>
+        <v>152.5666666666667</v>
       </c>
       <c r="D188" t="n">
-        <v>0.3046666666666666</v>
+        <v>0.3046666666666668</v>
       </c>
     </row>
     <row r="189">
@@ -3076,10 +3076,10 @@
         <v>1787</v>
       </c>
       <c r="C189" t="n">
-        <v>152.3833333333333</v>
+        <v>152.3833333333334</v>
       </c>
       <c r="D189" t="n">
-        <v>0.3043333333333333</v>
+        <v>0.3043333333333335</v>
       </c>
     </row>
     <row r="190">
@@ -3090,10 +3090,10 @@
         <v>1788</v>
       </c>
       <c r="C190" t="n">
-        <v>152.1999999999999</v>
+        <v>152.2</v>
       </c>
       <c r="D190" t="n">
-        <v>0.3039999999999999</v>
+        <v>0.3040000000000002</v>
       </c>
     </row>
     <row r="191">
@@ -3104,10 +3104,10 @@
         <v>1789</v>
       </c>
       <c r="C191" t="n">
-        <v>152.0166666666666</v>
+        <v>152.0166666666667</v>
       </c>
       <c r="D191" t="n">
-        <v>0.3036666666666666</v>
+        <v>0.3036666666666668</v>
       </c>
     </row>
     <row r="192">
@@ -3118,10 +3118,10 @@
         <v>1790</v>
       </c>
       <c r="C192" t="n">
-        <v>151.8333333333333</v>
+        <v>151.8333333333334</v>
       </c>
       <c r="D192" t="n">
-        <v>0.3033333333333333</v>
+        <v>0.3033333333333335</v>
       </c>
     </row>
     <row r="193">
@@ -3132,10 +3132,10 @@
         <v>1791</v>
       </c>
       <c r="C193" t="n">
-        <v>151.65</v>
+        <v>151.6500000000001</v>
       </c>
       <c r="D193" t="n">
-        <v>0.3029999999999999</v>
+        <v>0.3030000000000002</v>
       </c>
     </row>
     <row r="194">
@@ -3146,10 +3146,10 @@
         <v>1792</v>
       </c>
       <c r="C194" t="n">
-        <v>151.4666666666666</v>
+        <v>151.4666666666668</v>
       </c>
       <c r="D194" t="n">
-        <v>0.3026666666666666</v>
+        <v>0.3026666666666668</v>
       </c>
     </row>
     <row r="195">
@@ -3160,10 +3160,10 @@
         <v>1793</v>
       </c>
       <c r="C195" t="n">
-        <v>151.2833333333333</v>
+        <v>151.2833333333334</v>
       </c>
       <c r="D195" t="n">
-        <v>0.3023333333333333</v>
+        <v>0.3023333333333335</v>
       </c>
     </row>
     <row r="196">
@@ -3174,10 +3174,10 @@
         <v>1794</v>
       </c>
       <c r="C196" t="n">
-        <v>151.1</v>
+        <v>151.1000000000001</v>
       </c>
       <c r="D196" t="n">
-        <v>0.3019999999999999</v>
+        <v>0.3020000000000002</v>
       </c>
     </row>
     <row r="197">
@@ -3188,10 +3188,10 @@
         <v>1795</v>
       </c>
       <c r="C197" t="n">
-        <v>150.9166666666666</v>
+        <v>150.9166666666667</v>
       </c>
       <c r="D197" t="n">
-        <v>0.3016666666666666</v>
+        <v>0.3016666666666667</v>
       </c>
     </row>
     <row r="198">
@@ -3202,10 +3202,10 @@
         <v>1796</v>
       </c>
       <c r="C198" t="n">
-        <v>150.7333333333333</v>
+        <v>150.7333333333334</v>
       </c>
       <c r="D198" t="n">
-        <v>0.3013333333333333</v>
+        <v>0.3013333333333335</v>
       </c>
     </row>
     <row r="199">
@@ -3216,10 +3216,10 @@
         <v>1797</v>
       </c>
       <c r="C199" t="n">
-        <v>150.55</v>
+        <v>150.5500000000001</v>
       </c>
       <c r="D199" t="n">
-        <v>0.3009999999999999</v>
+        <v>0.3010000000000002</v>
       </c>
     </row>
     <row r="200">
@@ -3230,10 +3230,10 @@
         <v>1798</v>
       </c>
       <c r="C200" t="n">
-        <v>150.3666666666666</v>
+        <v>150.3666666666667</v>
       </c>
       <c r="D200" t="n">
-        <v>0.3006666666666666</v>
+        <v>0.3006666666666667</v>
       </c>
     </row>
     <row r="201">
@@ -3244,10 +3244,10 @@
         <v>1799</v>
       </c>
       <c r="C201" t="n">
-        <v>150.1833333333333</v>
+        <v>150.1833333333334</v>
       </c>
       <c r="D201" t="n">
-        <v>0.3003333333333333</v>
+        <v>0.3003333333333335</v>
       </c>
     </row>
     <row r="202">
@@ -6762,706 +6762,6 @@
       </c>
       <c r="D452" t="n">
         <v>0.2166666666666667</v>
-      </c>
-    </row>
-    <row r="453">
-      <c r="A453" s="1" t="n">
-        <v>451</v>
-      </c>
-      <c r="B453" t="n">
-        <v>2051</v>
-      </c>
-      <c r="C453" t="n">
-        <v>103.9833333333334</v>
-      </c>
-      <c r="D453" t="n">
-        <v>0.2163333333333334</v>
-      </c>
-    </row>
-    <row r="454">
-      <c r="A454" s="1" t="n">
-        <v>452</v>
-      </c>
-      <c r="B454" t="n">
-        <v>2052</v>
-      </c>
-      <c r="C454" t="n">
-        <v>103.8000000000001</v>
-      </c>
-      <c r="D454" t="n">
-        <v>0.2160000000000001</v>
-      </c>
-    </row>
-    <row r="455">
-      <c r="A455" s="1" t="n">
-        <v>453</v>
-      </c>
-      <c r="B455" t="n">
-        <v>2053</v>
-      </c>
-      <c r="C455" t="n">
-        <v>103.6166666666668</v>
-      </c>
-      <c r="D455" t="n">
-        <v>0.2156666666666667</v>
-      </c>
-    </row>
-    <row r="456">
-      <c r="A456" s="1" t="n">
-        <v>454</v>
-      </c>
-      <c r="B456" t="n">
-        <v>2054</v>
-      </c>
-      <c r="C456" t="n">
-        <v>103.4333333333334</v>
-      </c>
-      <c r="D456" t="n">
-        <v>0.2153333333333334</v>
-      </c>
-    </row>
-    <row r="457">
-      <c r="A457" s="1" t="n">
-        <v>455</v>
-      </c>
-      <c r="B457" t="n">
-        <v>2055</v>
-      </c>
-      <c r="C457" t="n">
-        <v>103.2500000000001</v>
-      </c>
-      <c r="D457" t="n">
-        <v>0.2150000000000001</v>
-      </c>
-    </row>
-    <row r="458">
-      <c r="A458" s="1" t="n">
-        <v>456</v>
-      </c>
-      <c r="B458" t="n">
-        <v>2056</v>
-      </c>
-      <c r="C458" t="n">
-        <v>103.0666666666667</v>
-      </c>
-      <c r="D458" t="n">
-        <v>0.2146666666666667</v>
-      </c>
-    </row>
-    <row r="459">
-      <c r="A459" s="1" t="n">
-        <v>457</v>
-      </c>
-      <c r="B459" t="n">
-        <v>2057</v>
-      </c>
-      <c r="C459" t="n">
-        <v>102.8833333333334</v>
-      </c>
-      <c r="D459" t="n">
-        <v>0.2143333333333334</v>
-      </c>
-    </row>
-    <row r="460">
-      <c r="A460" s="1" t="n">
-        <v>458</v>
-      </c>
-      <c r="B460" t="n">
-        <v>2058</v>
-      </c>
-      <c r="C460" t="n">
-        <v>102.7000000000001</v>
-      </c>
-      <c r="D460" t="n">
-        <v>0.2140000000000001</v>
-      </c>
-    </row>
-    <row r="461">
-      <c r="A461" s="1" t="n">
-        <v>459</v>
-      </c>
-      <c r="B461" t="n">
-        <v>2059</v>
-      </c>
-      <c r="C461" t="n">
-        <v>102.5166666666668</v>
-      </c>
-      <c r="D461" t="n">
-        <v>0.2136666666666667</v>
-      </c>
-    </row>
-    <row r="462">
-      <c r="A462" s="1" t="n">
-        <v>460</v>
-      </c>
-      <c r="B462" t="n">
-        <v>2060</v>
-      </c>
-      <c r="C462" t="n">
-        <v>102.3333333333334</v>
-      </c>
-      <c r="D462" t="n">
-        <v>0.2133333333333334</v>
-      </c>
-    </row>
-    <row r="463">
-      <c r="A463" s="1" t="n">
-        <v>461</v>
-      </c>
-      <c r="B463" t="n">
-        <v>2061</v>
-      </c>
-      <c r="C463" t="n">
-        <v>102.1500000000001</v>
-      </c>
-      <c r="D463" t="n">
-        <v>0.2130000000000001</v>
-      </c>
-    </row>
-    <row r="464">
-      <c r="A464" s="1" t="n">
-        <v>462</v>
-      </c>
-      <c r="B464" t="n">
-        <v>2062</v>
-      </c>
-      <c r="C464" t="n">
-        <v>101.9666666666668</v>
-      </c>
-      <c r="D464" t="n">
-        <v>0.2126666666666667</v>
-      </c>
-    </row>
-    <row r="465">
-      <c r="A465" s="1" t="n">
-        <v>463</v>
-      </c>
-      <c r="B465" t="n">
-        <v>2063</v>
-      </c>
-      <c r="C465" t="n">
-        <v>101.7833333333334</v>
-      </c>
-      <c r="D465" t="n">
-        <v>0.2123333333333334</v>
-      </c>
-    </row>
-    <row r="466">
-      <c r="A466" s="1" t="n">
-        <v>464</v>
-      </c>
-      <c r="B466" t="n">
-        <v>2064</v>
-      </c>
-      <c r="C466" t="n">
-        <v>101.6000000000001</v>
-      </c>
-      <c r="D466" t="n">
-        <v>0.2120000000000001</v>
-      </c>
-    </row>
-    <row r="467">
-      <c r="A467" s="1" t="n">
-        <v>465</v>
-      </c>
-      <c r="B467" t="n">
-        <v>2065</v>
-      </c>
-      <c r="C467" t="n">
-        <v>101.4166666666668</v>
-      </c>
-      <c r="D467" t="n">
-        <v>0.2116666666666667</v>
-      </c>
-    </row>
-    <row r="468">
-      <c r="A468" s="1" t="n">
-        <v>466</v>
-      </c>
-      <c r="B468" t="n">
-        <v>2066</v>
-      </c>
-      <c r="C468" t="n">
-        <v>101.2333333333334</v>
-      </c>
-      <c r="D468" t="n">
-        <v>0.2113333333333334</v>
-      </c>
-    </row>
-    <row r="469">
-      <c r="A469" s="1" t="n">
-        <v>467</v>
-      </c>
-      <c r="B469" t="n">
-        <v>2067</v>
-      </c>
-      <c r="C469" t="n">
-        <v>101.0500000000001</v>
-      </c>
-      <c r="D469" t="n">
-        <v>0.2110000000000001</v>
-      </c>
-    </row>
-    <row r="470">
-      <c r="A470" s="1" t="n">
-        <v>468</v>
-      </c>
-      <c r="B470" t="n">
-        <v>2068</v>
-      </c>
-      <c r="C470" t="n">
-        <v>100.8666666666668</v>
-      </c>
-      <c r="D470" t="n">
-        <v>0.2106666666666668</v>
-      </c>
-    </row>
-    <row r="471">
-      <c r="A471" s="1" t="n">
-        <v>469</v>
-      </c>
-      <c r="B471" t="n">
-        <v>2069</v>
-      </c>
-      <c r="C471" t="n">
-        <v>100.6833333333334</v>
-      </c>
-      <c r="D471" t="n">
-        <v>0.2103333333333334</v>
-      </c>
-    </row>
-    <row r="472">
-      <c r="A472" s="1" t="n">
-        <v>470</v>
-      </c>
-      <c r="B472" t="n">
-        <v>2070</v>
-      </c>
-      <c r="C472" t="n">
-        <v>100.5000000000001</v>
-      </c>
-      <c r="D472" t="n">
-        <v>0.2100000000000001</v>
-      </c>
-    </row>
-    <row r="473">
-      <c r="A473" s="1" t="n">
-        <v>471</v>
-      </c>
-      <c r="B473" t="n">
-        <v>2071</v>
-      </c>
-      <c r="C473" t="n">
-        <v>100.3166666666668</v>
-      </c>
-      <c r="D473" t="n">
-        <v>0.2096666666666668</v>
-      </c>
-    </row>
-    <row r="474">
-      <c r="A474" s="1" t="n">
-        <v>472</v>
-      </c>
-      <c r="B474" t="n">
-        <v>2072</v>
-      </c>
-      <c r="C474" t="n">
-        <v>100.1333333333334</v>
-      </c>
-      <c r="D474" t="n">
-        <v>0.2093333333333334</v>
-      </c>
-    </row>
-    <row r="475">
-      <c r="A475" s="1" t="n">
-        <v>473</v>
-      </c>
-      <c r="B475" t="n">
-        <v>2073</v>
-      </c>
-      <c r="C475" t="n">
-        <v>99.9500000000001</v>
-      </c>
-      <c r="D475" t="n">
-        <v>0.2090000000000001</v>
-      </c>
-    </row>
-    <row r="476">
-      <c r="A476" s="1" t="n">
-        <v>474</v>
-      </c>
-      <c r="B476" t="n">
-        <v>2074</v>
-      </c>
-      <c r="C476" t="n">
-        <v>99.76666666666677</v>
-      </c>
-      <c r="D476" t="n">
-        <v>0.2086666666666668</v>
-      </c>
-    </row>
-    <row r="477">
-      <c r="A477" s="1" t="n">
-        <v>475</v>
-      </c>
-      <c r="B477" t="n">
-        <v>2075</v>
-      </c>
-      <c r="C477" t="n">
-        <v>99.58333333333343</v>
-      </c>
-      <c r="D477" t="n">
-        <v>0.2083333333333334</v>
-      </c>
-    </row>
-    <row r="478">
-      <c r="A478" s="1" t="n">
-        <v>476</v>
-      </c>
-      <c r="B478" t="n">
-        <v>2076</v>
-      </c>
-      <c r="C478" t="n">
-        <v>99.40000000000009</v>
-      </c>
-      <c r="D478" t="n">
-        <v>0.2080000000000001</v>
-      </c>
-    </row>
-    <row r="479">
-      <c r="A479" s="1" t="n">
-        <v>477</v>
-      </c>
-      <c r="B479" t="n">
-        <v>2077</v>
-      </c>
-      <c r="C479" t="n">
-        <v>99.21666666666675</v>
-      </c>
-      <c r="D479" t="n">
-        <v>0.2076666666666667</v>
-      </c>
-    </row>
-    <row r="480">
-      <c r="A480" s="1" t="n">
-        <v>478</v>
-      </c>
-      <c r="B480" t="n">
-        <v>2078</v>
-      </c>
-      <c r="C480" t="n">
-        <v>99.03333333333343</v>
-      </c>
-      <c r="D480" t="n">
-        <v>0.2073333333333334</v>
-      </c>
-    </row>
-    <row r="481">
-      <c r="A481" s="1" t="n">
-        <v>479</v>
-      </c>
-      <c r="B481" t="n">
-        <v>2079</v>
-      </c>
-      <c r="C481" t="n">
-        <v>98.85000000000009</v>
-      </c>
-      <c r="D481" t="n">
-        <v>0.2070000000000001</v>
-      </c>
-    </row>
-    <row r="482">
-      <c r="A482" s="1" t="n">
-        <v>480</v>
-      </c>
-      <c r="B482" t="n">
-        <v>2080</v>
-      </c>
-      <c r="C482" t="n">
-        <v>98.66666666666677</v>
-      </c>
-      <c r="D482" t="n">
-        <v>0.2066666666666667</v>
-      </c>
-    </row>
-    <row r="483">
-      <c r="A483" s="1" t="n">
-        <v>481</v>
-      </c>
-      <c r="B483" t="n">
-        <v>2081</v>
-      </c>
-      <c r="C483" t="n">
-        <v>98.48333333333343</v>
-      </c>
-      <c r="D483" t="n">
-        <v>0.2063333333333334</v>
-      </c>
-    </row>
-    <row r="484">
-      <c r="A484" s="1" t="n">
-        <v>482</v>
-      </c>
-      <c r="B484" t="n">
-        <v>2082</v>
-      </c>
-      <c r="C484" t="n">
-        <v>98.3000000000001</v>
-      </c>
-      <c r="D484" t="n">
-        <v>0.2060000000000001</v>
-      </c>
-    </row>
-    <row r="485">
-      <c r="A485" s="1" t="n">
-        <v>483</v>
-      </c>
-      <c r="B485" t="n">
-        <v>2083</v>
-      </c>
-      <c r="C485" t="n">
-        <v>98.11666666666676</v>
-      </c>
-      <c r="D485" t="n">
-        <v>0.2056666666666667</v>
-      </c>
-    </row>
-    <row r="486">
-      <c r="A486" s="1" t="n">
-        <v>484</v>
-      </c>
-      <c r="B486" t="n">
-        <v>2084</v>
-      </c>
-      <c r="C486" t="n">
-        <v>97.93333333333342</v>
-      </c>
-      <c r="D486" t="n">
-        <v>0.2053333333333334</v>
-      </c>
-    </row>
-    <row r="487">
-      <c r="A487" s="1" t="n">
-        <v>485</v>
-      </c>
-      <c r="B487" t="n">
-        <v>2085</v>
-      </c>
-      <c r="C487" t="n">
-        <v>97.7500000000001</v>
-      </c>
-      <c r="D487" t="n">
-        <v>0.2050000000000001</v>
-      </c>
-    </row>
-    <row r="488">
-      <c r="A488" s="1" t="n">
-        <v>486</v>
-      </c>
-      <c r="B488" t="n">
-        <v>2086</v>
-      </c>
-      <c r="C488" t="n">
-        <v>97.56666666666676</v>
-      </c>
-      <c r="D488" t="n">
-        <v>0.2046666666666667</v>
-      </c>
-    </row>
-    <row r="489">
-      <c r="A489" s="1" t="n">
-        <v>487</v>
-      </c>
-      <c r="B489" t="n">
-        <v>2087</v>
-      </c>
-      <c r="C489" t="n">
-        <v>97.38333333333344</v>
-      </c>
-      <c r="D489" t="n">
-        <v>0.2043333333333334</v>
-      </c>
-    </row>
-    <row r="490">
-      <c r="A490" s="1" t="n">
-        <v>488</v>
-      </c>
-      <c r="B490" t="n">
-        <v>2088</v>
-      </c>
-      <c r="C490" t="n">
-        <v>97.2000000000001</v>
-      </c>
-      <c r="D490" t="n">
-        <v>0.2040000000000001</v>
-      </c>
-    </row>
-    <row r="491">
-      <c r="A491" s="1" t="n">
-        <v>489</v>
-      </c>
-      <c r="B491" t="n">
-        <v>2089</v>
-      </c>
-      <c r="C491" t="n">
-        <v>97.01666666666677</v>
-      </c>
-      <c r="D491" t="n">
-        <v>0.2036666666666668</v>
-      </c>
-    </row>
-    <row r="492">
-      <c r="A492" s="1" t="n">
-        <v>490</v>
-      </c>
-      <c r="B492" t="n">
-        <v>2090</v>
-      </c>
-      <c r="C492" t="n">
-        <v>96.83333333333343</v>
-      </c>
-      <c r="D492" t="n">
-        <v>0.2033333333333334</v>
-      </c>
-    </row>
-    <row r="493">
-      <c r="A493" s="1" t="n">
-        <v>491</v>
-      </c>
-      <c r="B493" t="n">
-        <v>2091</v>
-      </c>
-      <c r="C493" t="n">
-        <v>96.65000000000009</v>
-      </c>
-      <c r="D493" t="n">
-        <v>0.2030000000000001</v>
-      </c>
-    </row>
-    <row r="494">
-      <c r="A494" s="1" t="n">
-        <v>492</v>
-      </c>
-      <c r="B494" t="n">
-        <v>2092</v>
-      </c>
-      <c r="C494" t="n">
-        <v>96.46666666666677</v>
-      </c>
-      <c r="D494" t="n">
-        <v>0.2026666666666668</v>
-      </c>
-    </row>
-    <row r="495">
-      <c r="A495" s="1" t="n">
-        <v>493</v>
-      </c>
-      <c r="B495" t="n">
-        <v>2093</v>
-      </c>
-      <c r="C495" t="n">
-        <v>96.28333333333345</v>
-      </c>
-      <c r="D495" t="n">
-        <v>0.2023333333333334</v>
-      </c>
-    </row>
-    <row r="496">
-      <c r="A496" s="1" t="n">
-        <v>494</v>
-      </c>
-      <c r="B496" t="n">
-        <v>2094</v>
-      </c>
-      <c r="C496" t="n">
-        <v>96.10000000000011</v>
-      </c>
-      <c r="D496" t="n">
-        <v>0.2020000000000001</v>
-      </c>
-    </row>
-    <row r="497">
-      <c r="A497" s="1" t="n">
-        <v>495</v>
-      </c>
-      <c r="B497" t="n">
-        <v>2095</v>
-      </c>
-      <c r="C497" t="n">
-        <v>95.91666666666677</v>
-      </c>
-      <c r="D497" t="n">
-        <v>0.2016666666666668</v>
-      </c>
-    </row>
-    <row r="498">
-      <c r="A498" s="1" t="n">
-        <v>496</v>
-      </c>
-      <c r="B498" t="n">
-        <v>2096</v>
-      </c>
-      <c r="C498" t="n">
-        <v>95.73333333333343</v>
-      </c>
-      <c r="D498" t="n">
-        <v>0.2013333333333334</v>
-      </c>
-    </row>
-    <row r="499">
-      <c r="A499" s="1" t="n">
-        <v>497</v>
-      </c>
-      <c r="B499" t="n">
-        <v>2097</v>
-      </c>
-      <c r="C499" t="n">
-        <v>95.5500000000001</v>
-      </c>
-      <c r="D499" t="n">
-        <v>0.2010000000000001</v>
-      </c>
-    </row>
-    <row r="500">
-      <c r="A500" s="1" t="n">
-        <v>498</v>
-      </c>
-      <c r="B500" t="n">
-        <v>2098</v>
-      </c>
-      <c r="C500" t="n">
-        <v>95.36666666666676</v>
-      </c>
-      <c r="D500" t="n">
-        <v>0.2006666666666668</v>
-      </c>
-    </row>
-    <row r="501">
-      <c r="A501" s="1" t="n">
-        <v>499</v>
-      </c>
-      <c r="B501" t="n">
-        <v>2099</v>
-      </c>
-      <c r="C501" t="n">
-        <v>95.18333333333344</v>
-      </c>
-      <c r="D501" t="n">
-        <v>0.2003333333333334</v>
-      </c>
-    </row>
-    <row r="502">
-      <c r="A502" s="1" t="n">
-        <v>500</v>
-      </c>
-      <c r="B502" t="n">
-        <v>2100</v>
-      </c>
-      <c r="C502" t="n">
-        <v>95.00000000000011</v>
-      </c>
-      <c r="D502" t="n">
-        <v>0.2000000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make sigma to std_dev
</commit_message>
<xml_diff>
--- a/Data/regression_data/Dwelling_Lifetime/regression_Dwelling_Lifetime.xlsx
+++ b/Data/regression_data/Dwelling_Lifetime/regression_Dwelling_Lifetime.xlsx
@@ -461,7 +461,7 @@
         <v>186.6666666666667</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3666666666666667</v>
+        <v>62.31041666666667</v>
       </c>
     </row>
     <row r="3">
@@ -475,7 +475,7 @@
         <v>186.4833333333333</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3663333333333334</v>
+        <v>62.22069444444443</v>
       </c>
     </row>
     <row r="4">
@@ -489,7 +489,7 @@
         <v>186.3</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3660000000000001</v>
+        <v>62.1309722222222</v>
       </c>
     </row>
     <row r="5">
@@ -503,7 +503,7 @@
         <v>186.1166666666667</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3656666666666667</v>
+        <v>62.04124999999999</v>
       </c>
     </row>
     <row r="6">
@@ -517,7 +517,7 @@
         <v>185.9333333333333</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3653333333333334</v>
+        <v>61.95152777777776</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>185.75</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3650000000000001</v>
+        <v>61.86180555555555</v>
       </c>
     </row>
     <row r="8">
@@ -545,7 +545,7 @@
         <v>185.5666666666667</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3646666666666667</v>
+        <v>61.77208333333331</v>
       </c>
     </row>
     <row r="9">
@@ -559,7 +559,7 @@
         <v>185.3833333333333</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3643333333333334</v>
+        <v>61.68236111111111</v>
       </c>
     </row>
     <row r="10">
@@ -573,7 +573,7 @@
         <v>185.2</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3640000000000001</v>
+        <v>61.59263888888887</v>
       </c>
     </row>
     <row r="11">
@@ -587,7 +587,7 @@
         <v>185.0166666666667</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3636666666666667</v>
+        <v>61.50291666666666</v>
       </c>
     </row>
     <row r="12">
@@ -601,7 +601,7 @@
         <v>184.8333333333334</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3633333333333334</v>
+        <v>61.41319444444443</v>
       </c>
     </row>
     <row r="13">
@@ -615,7 +615,7 @@
         <v>184.65</v>
       </c>
       <c r="D13" t="n">
-        <v>0.3630000000000001</v>
+        <v>61.32347222222222</v>
       </c>
     </row>
     <row r="14">
@@ -629,7 +629,7 @@
         <v>184.4666666666667</v>
       </c>
       <c r="D14" t="n">
-        <v>0.3626666666666667</v>
+        <v>61.23374999999999</v>
       </c>
     </row>
     <row r="15">
@@ -643,7 +643,7 @@
         <v>184.2833333333334</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3623333333333334</v>
+        <v>61.14402777777778</v>
       </c>
     </row>
     <row r="16">
@@ -657,7 +657,7 @@
         <v>184.1</v>
       </c>
       <c r="D16" t="n">
-        <v>0.3620000000000001</v>
+        <v>61.05430555555554</v>
       </c>
     </row>
     <row r="17">
@@ -671,7 +671,7 @@
         <v>183.9166666666667</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3616666666666668</v>
+        <v>60.96458333333334</v>
       </c>
     </row>
     <row r="18">
@@ -685,7 +685,7 @@
         <v>183.7333333333333</v>
       </c>
       <c r="D18" t="n">
-        <v>0.3613333333333334</v>
+        <v>60.8748611111111</v>
       </c>
     </row>
     <row r="19">
@@ -699,7 +699,7 @@
         <v>183.55</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3610000000000001</v>
+        <v>60.78513888888887</v>
       </c>
     </row>
     <row r="20">
@@ -713,7 +713,7 @@
         <v>183.3666666666667</v>
       </c>
       <c r="D20" t="n">
-        <v>0.3606666666666668</v>
+        <v>60.69541666666666</v>
       </c>
     </row>
     <row r="21">
@@ -727,7 +727,7 @@
         <v>183.1833333333333</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3603333333333334</v>
+        <v>60.60569444444442</v>
       </c>
     </row>
     <row r="22">
@@ -741,7 +741,7 @@
         <v>183</v>
       </c>
       <c r="D22" t="n">
-        <v>0.3600000000000001</v>
+        <v>60.51597222222222</v>
       </c>
     </row>
     <row r="23">
@@ -755,7 +755,7 @@
         <v>182.8166666666667</v>
       </c>
       <c r="D23" t="n">
-        <v>0.3596666666666668</v>
+        <v>60.42624999999998</v>
       </c>
     </row>
     <row r="24">
@@ -769,7 +769,7 @@
         <v>182.6333333333333</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3593333333333334</v>
+        <v>60.33652777777777</v>
       </c>
     </row>
     <row r="25">
@@ -783,7 +783,7 @@
         <v>182.45</v>
       </c>
       <c r="D25" t="n">
-        <v>0.3590000000000001</v>
+        <v>60.24680555555554</v>
       </c>
     </row>
     <row r="26">
@@ -797,7 +797,7 @@
         <v>182.2666666666667</v>
       </c>
       <c r="D26" t="n">
-        <v>0.3586666666666668</v>
+        <v>60.15708333333333</v>
       </c>
     </row>
     <row r="27">
@@ -811,7 +811,7 @@
         <v>182.0833333333334</v>
       </c>
       <c r="D27" t="n">
-        <v>0.3583333333333334</v>
+        <v>60.0673611111111</v>
       </c>
     </row>
     <row r="28">
@@ -825,7 +825,7 @@
         <v>181.9</v>
       </c>
       <c r="D28" t="n">
-        <v>0.3580000000000001</v>
+        <v>59.97763888888889</v>
       </c>
     </row>
     <row r="29">
@@ -839,7 +839,7 @@
         <v>181.7166666666667</v>
       </c>
       <c r="D29" t="n">
-        <v>0.3576666666666668</v>
+        <v>59.88791666666665</v>
       </c>
     </row>
     <row r="30">
@@ -853,7 +853,7 @@
         <v>181.5333333333334</v>
       </c>
       <c r="D30" t="n">
-        <v>0.3573333333333334</v>
+        <v>59.79819444444445</v>
       </c>
     </row>
     <row r="31">
@@ -867,7 +867,7 @@
         <v>181.35</v>
       </c>
       <c r="D31" t="n">
-        <v>0.3570000000000001</v>
+        <v>59.70847222222221</v>
       </c>
     </row>
     <row r="32">
@@ -881,7 +881,7 @@
         <v>181.1666666666667</v>
       </c>
       <c r="D32" t="n">
-        <v>0.3566666666666668</v>
+        <v>59.61874999999998</v>
       </c>
     </row>
     <row r="33">
@@ -895,7 +895,7 @@
         <v>180.9833333333333</v>
       </c>
       <c r="D33" t="n">
-        <v>0.3563333333333334</v>
+        <v>59.52902777777777</v>
       </c>
     </row>
     <row r="34">
@@ -909,7 +909,7 @@
         <v>180.8</v>
       </c>
       <c r="D34" t="n">
-        <v>0.3560000000000001</v>
+        <v>59.43930555555553</v>
       </c>
     </row>
     <row r="35">
@@ -923,7 +923,7 @@
         <v>180.6166666666667</v>
       </c>
       <c r="D35" t="n">
-        <v>0.3556666666666668</v>
+        <v>59.34958333333333</v>
       </c>
     </row>
     <row r="36">
@@ -937,7 +937,7 @@
         <v>180.4333333333333</v>
       </c>
       <c r="D36" t="n">
-        <v>0.3553333333333334</v>
+        <v>59.25986111111109</v>
       </c>
     </row>
     <row r="37">
@@ -951,7 +951,7 @@
         <v>180.25</v>
       </c>
       <c r="D37" t="n">
-        <v>0.3550000000000001</v>
+        <v>59.17013888888889</v>
       </c>
     </row>
     <row r="38">
@@ -965,7 +965,7 @@
         <v>180.0666666666667</v>
       </c>
       <c r="D38" t="n">
-        <v>0.3546666666666668</v>
+        <v>59.08041666666665</v>
       </c>
     </row>
     <row r="39">
@@ -979,7 +979,7 @@
         <v>179.8833333333333</v>
       </c>
       <c r="D39" t="n">
-        <v>0.3543333333333334</v>
+        <v>58.99069444444444</v>
       </c>
     </row>
     <row r="40">
@@ -993,7 +993,7 @@
         <v>179.7</v>
       </c>
       <c r="D40" t="n">
-        <v>0.3540000000000001</v>
+        <v>58.90097222222221</v>
       </c>
     </row>
     <row r="41">
@@ -1007,7 +1007,7 @@
         <v>179.5166666666667</v>
       </c>
       <c r="D41" t="n">
-        <v>0.3536666666666668</v>
+        <v>58.81125</v>
       </c>
     </row>
     <row r="42">
@@ -1021,7 +1021,7 @@
         <v>179.3333333333334</v>
       </c>
       <c r="D42" t="n">
-        <v>0.3533333333333334</v>
+        <v>58.72152777777777</v>
       </c>
     </row>
     <row r="43">
@@ -1035,7 +1035,7 @@
         <v>179.15</v>
       </c>
       <c r="D43" t="n">
-        <v>0.3530000000000001</v>
+        <v>58.63180555555556</v>
       </c>
     </row>
     <row r="44">
@@ -1049,7 +1049,7 @@
         <v>178.9666666666667</v>
       </c>
       <c r="D44" t="n">
-        <v>0.3526666666666668</v>
+        <v>58.54208333333332</v>
       </c>
     </row>
     <row r="45">
@@ -1063,7 +1063,7 @@
         <v>178.7833333333334</v>
       </c>
       <c r="D45" t="n">
-        <v>0.3523333333333334</v>
+        <v>58.45236111111112</v>
       </c>
     </row>
     <row r="46">
@@ -1077,7 +1077,7 @@
         <v>178.6</v>
       </c>
       <c r="D46" t="n">
-        <v>0.3520000000000001</v>
+        <v>58.36263888888888</v>
       </c>
     </row>
     <row r="47">
@@ -1091,7 +1091,7 @@
         <v>178.4166666666667</v>
       </c>
       <c r="D47" t="n">
-        <v>0.3516666666666668</v>
+        <v>58.27291666666665</v>
       </c>
     </row>
     <row r="48">
@@ -1105,7 +1105,7 @@
         <v>178.2333333333333</v>
       </c>
       <c r="D48" t="n">
-        <v>0.3513333333333334</v>
+        <v>58.18319444444444</v>
       </c>
     </row>
     <row r="49">
@@ -1119,7 +1119,7 @@
         <v>178.05</v>
       </c>
       <c r="D49" t="n">
-        <v>0.3510000000000001</v>
+        <v>58.0934722222222</v>
       </c>
     </row>
     <row r="50">
@@ -1133,7 +1133,7 @@
         <v>177.8666666666667</v>
       </c>
       <c r="D50" t="n">
-        <v>0.3506666666666668</v>
+        <v>58.00375</v>
       </c>
     </row>
     <row r="51">
@@ -1147,7 +1147,7 @@
         <v>177.6833333333333</v>
       </c>
       <c r="D51" t="n">
-        <v>0.3503333333333334</v>
+        <v>57.91402777777776</v>
       </c>
     </row>
     <row r="52">
@@ -1161,7 +1161,7 @@
         <v>177.5</v>
       </c>
       <c r="D52" t="n">
-        <v>0.3500000000000001</v>
+        <v>57.82430555555555</v>
       </c>
     </row>
     <row r="53">
@@ -1175,7 +1175,7 @@
         <v>177.3166666666667</v>
       </c>
       <c r="D53" t="n">
-        <v>0.3496666666666668</v>
+        <v>57.73458333333332</v>
       </c>
     </row>
     <row r="54">
@@ -1189,7 +1189,7 @@
         <v>177.1333333333334</v>
       </c>
       <c r="D54" t="n">
-        <v>0.3493333333333334</v>
+        <v>57.64486111111111</v>
       </c>
     </row>
     <row r="55">
@@ -1203,7 +1203,7 @@
         <v>176.95</v>
       </c>
       <c r="D55" t="n">
-        <v>0.3490000000000001</v>
+        <v>57.55513888888888</v>
       </c>
     </row>
     <row r="56">
@@ -1217,7 +1217,7 @@
         <v>176.7666666666667</v>
       </c>
       <c r="D56" t="n">
-        <v>0.3486666666666668</v>
+        <v>57.46541666666667</v>
       </c>
     </row>
     <row r="57">
@@ -1231,7 +1231,7 @@
         <v>176.5833333333334</v>
       </c>
       <c r="D57" t="n">
-        <v>0.3483333333333334</v>
+        <v>57.37569444444443</v>
       </c>
     </row>
     <row r="58">
@@ -1245,7 +1245,7 @@
         <v>176.4</v>
       </c>
       <c r="D58" t="n">
-        <v>0.3480000000000001</v>
+        <v>57.28597222222223</v>
       </c>
     </row>
     <row r="59">
@@ -1259,7 +1259,7 @@
         <v>176.2166666666667</v>
       </c>
       <c r="D59" t="n">
-        <v>0.3476666666666668</v>
+        <v>57.19624999999999</v>
       </c>
     </row>
     <row r="60">
@@ -1273,7 +1273,7 @@
         <v>176.0333333333334</v>
       </c>
       <c r="D60" t="n">
-        <v>0.3473333333333334</v>
+        <v>57.10652777777779</v>
       </c>
     </row>
     <row r="61">
@@ -1287,7 +1287,7 @@
         <v>175.85</v>
       </c>
       <c r="D61" t="n">
-        <v>0.3470000000000001</v>
+        <v>57.01680555555555</v>
       </c>
     </row>
     <row r="62">
@@ -1301,7 +1301,7 @@
         <v>175.6666666666667</v>
       </c>
       <c r="D62" t="n">
-        <v>0.3466666666666668</v>
+        <v>56.92708333333331</v>
       </c>
     </row>
     <row r="63">
@@ -1315,7 +1315,7 @@
         <v>175.4833333333333</v>
       </c>
       <c r="D63" t="n">
-        <v>0.3463333333333334</v>
+        <v>56.83736111111111</v>
       </c>
     </row>
     <row r="64">
@@ -1329,7 +1329,7 @@
         <v>175.3</v>
       </c>
       <c r="D64" t="n">
-        <v>0.3460000000000001</v>
+        <v>56.74763888888887</v>
       </c>
     </row>
     <row r="65">
@@ -1343,7 +1343,7 @@
         <v>175.1166666666667</v>
       </c>
       <c r="D65" t="n">
-        <v>0.3456666666666668</v>
+        <v>56.65791666666667</v>
       </c>
     </row>
     <row r="66">
@@ -1357,7 +1357,7 @@
         <v>174.9333333333333</v>
       </c>
       <c r="D66" t="n">
-        <v>0.3453333333333334</v>
+        <v>56.56819444444443</v>
       </c>
     </row>
     <row r="67">
@@ -1371,7 +1371,7 @@
         <v>174.7500000000001</v>
       </c>
       <c r="D67" t="n">
-        <v>0.3450000000000001</v>
+        <v>56.47847222222222</v>
       </c>
     </row>
     <row r="68">
@@ -1385,7 +1385,7 @@
         <v>174.5666666666667</v>
       </c>
       <c r="D68" t="n">
-        <v>0.3446666666666668</v>
+        <v>56.38874999999999</v>
       </c>
     </row>
     <row r="69">
@@ -1399,7 +1399,7 @@
         <v>174.3833333333334</v>
       </c>
       <c r="D69" t="n">
-        <v>0.3443333333333334</v>
+        <v>56.29902777777778</v>
       </c>
     </row>
     <row r="70">
@@ -1413,7 +1413,7 @@
         <v>174.2</v>
       </c>
       <c r="D70" t="n">
-        <v>0.3440000000000001</v>
+        <v>56.20930555555555</v>
       </c>
     </row>
     <row r="71">
@@ -1427,7 +1427,7 @@
         <v>174.0166666666667</v>
       </c>
       <c r="D71" t="n">
-        <v>0.3436666666666668</v>
+        <v>56.11958333333334</v>
       </c>
     </row>
     <row r="72">
@@ -1441,7 +1441,7 @@
         <v>173.8333333333334</v>
       </c>
       <c r="D72" t="n">
-        <v>0.3433333333333334</v>
+        <v>56.0298611111111</v>
       </c>
     </row>
     <row r="73">
@@ -1455,7 +1455,7 @@
         <v>173.65</v>
       </c>
       <c r="D73" t="n">
-        <v>0.3430000000000001</v>
+        <v>55.9401388888889</v>
       </c>
     </row>
     <row r="74">
@@ -1469,7 +1469,7 @@
         <v>173.4666666666667</v>
       </c>
       <c r="D74" t="n">
-        <v>0.3426666666666668</v>
+        <v>55.85041666666666</v>
       </c>
     </row>
     <row r="75">
@@ -1483,7 +1483,7 @@
         <v>173.2833333333334</v>
       </c>
       <c r="D75" t="n">
-        <v>0.3423333333333334</v>
+        <v>55.76069444444445</v>
       </c>
     </row>
     <row r="76">
@@ -1497,7 +1497,7 @@
         <v>173.1</v>
       </c>
       <c r="D76" t="n">
-        <v>0.3420000000000001</v>
+        <v>55.67097222222222</v>
       </c>
     </row>
     <row r="77">
@@ -1511,7 +1511,7 @@
         <v>172.9166666666667</v>
       </c>
       <c r="D77" t="n">
-        <v>0.3416666666666668</v>
+        <v>55.58124999999998</v>
       </c>
     </row>
     <row r="78">
@@ -1525,7 +1525,7 @@
         <v>172.7333333333333</v>
       </c>
       <c r="D78" t="n">
-        <v>0.3413333333333334</v>
+        <v>55.49152777777778</v>
       </c>
     </row>
     <row r="79">
@@ -1539,7 +1539,7 @@
         <v>172.55</v>
       </c>
       <c r="D79" t="n">
-        <v>0.3410000000000001</v>
+        <v>55.40180555555554</v>
       </c>
     </row>
     <row r="80">
@@ -1553,7 +1553,7 @@
         <v>172.3666666666667</v>
       </c>
       <c r="D80" t="n">
-        <v>0.3406666666666668</v>
+        <v>55.31208333333333</v>
       </c>
     </row>
     <row r="81">
@@ -1567,7 +1567,7 @@
         <v>172.1833333333334</v>
       </c>
       <c r="D81" t="n">
-        <v>0.3403333333333334</v>
+        <v>55.2223611111111</v>
       </c>
     </row>
     <row r="82">
@@ -1581,7 +1581,7 @@
         <v>172.0000000000001</v>
       </c>
       <c r="D82" t="n">
-        <v>0.3400000000000001</v>
+        <v>55.13263888888889</v>
       </c>
     </row>
     <row r="83">
@@ -1595,7 +1595,7 @@
         <v>171.8166666666667</v>
       </c>
       <c r="D83" t="n">
-        <v>0.3396666666666668</v>
+        <v>55.04291666666666</v>
       </c>
     </row>
     <row r="84">
@@ -1609,7 +1609,7 @@
         <v>171.6333333333334</v>
       </c>
       <c r="D84" t="n">
-        <v>0.3393333333333334</v>
+        <v>54.95319444444445</v>
       </c>
     </row>
     <row r="85">
@@ -1623,7 +1623,7 @@
         <v>171.45</v>
       </c>
       <c r="D85" t="n">
-        <v>0.3390000000000001</v>
+        <v>54.86347222222221</v>
       </c>
     </row>
     <row r="86">
@@ -1637,7 +1637,7 @@
         <v>171.2666666666667</v>
       </c>
       <c r="D86" t="n">
-        <v>0.3386666666666668</v>
+        <v>54.77375000000001</v>
       </c>
     </row>
     <row r="87">
@@ -1651,7 +1651,7 @@
         <v>171.0833333333334</v>
       </c>
       <c r="D87" t="n">
-        <v>0.3383333333333334</v>
+        <v>54.68402777777777</v>
       </c>
     </row>
     <row r="88">
@@ -1665,7 +1665,7 @@
         <v>170.9</v>
       </c>
       <c r="D88" t="n">
-        <v>0.3380000000000001</v>
+        <v>54.59430555555556</v>
       </c>
     </row>
     <row r="89">
@@ -1679,7 +1679,7 @@
         <v>170.7166666666667</v>
       </c>
       <c r="D89" t="n">
-        <v>0.3376666666666668</v>
+        <v>54.50458333333333</v>
       </c>
     </row>
     <row r="90">
@@ -1693,7 +1693,7 @@
         <v>170.5333333333334</v>
       </c>
       <c r="D90" t="n">
-        <v>0.3373333333333334</v>
+        <v>54.41486111111109</v>
       </c>
     </row>
     <row r="91">
@@ -1707,7 +1707,7 @@
         <v>170.35</v>
       </c>
       <c r="D91" t="n">
-        <v>0.3370000000000001</v>
+        <v>54.32513888888889</v>
       </c>
     </row>
     <row r="92">
@@ -1721,7 +1721,7 @@
         <v>170.1666666666667</v>
       </c>
       <c r="D92" t="n">
-        <v>0.3366666666666668</v>
+        <v>54.23541666666665</v>
       </c>
     </row>
     <row r="93">
@@ -1735,7 +1735,7 @@
         <v>169.9833333333333</v>
       </c>
       <c r="D93" t="n">
-        <v>0.3363333333333334</v>
+        <v>54.14569444444444</v>
       </c>
     </row>
     <row r="94">
@@ -1749,7 +1749,7 @@
         <v>169.8</v>
       </c>
       <c r="D94" t="n">
-        <v>0.3360000000000001</v>
+        <v>54.05597222222221</v>
       </c>
     </row>
     <row r="95">
@@ -1763,7 +1763,7 @@
         <v>169.6166666666667</v>
       </c>
       <c r="D95" t="n">
-        <v>0.3356666666666668</v>
+        <v>53.96625</v>
       </c>
     </row>
     <row r="96">
@@ -1777,7 +1777,7 @@
         <v>169.4333333333334</v>
       </c>
       <c r="D96" t="n">
-        <v>0.3353333333333335</v>
+        <v>53.87652777777777</v>
       </c>
     </row>
     <row r="97">
@@ -1791,7 +1791,7 @@
         <v>169.2500000000001</v>
       </c>
       <c r="D97" t="n">
-        <v>0.3350000000000001</v>
+        <v>53.78680555555556</v>
       </c>
     </row>
     <row r="98">
@@ -1805,7 +1805,7 @@
         <v>169.0666666666667</v>
       </c>
       <c r="D98" t="n">
-        <v>0.3346666666666668</v>
+        <v>53.69708333333332</v>
       </c>
     </row>
     <row r="99">
@@ -1819,7 +1819,7 @@
         <v>168.8833333333334</v>
       </c>
       <c r="D99" t="n">
-        <v>0.3343333333333335</v>
+        <v>53.60736111111112</v>
       </c>
     </row>
     <row r="100">
@@ -1833,7 +1833,7 @@
         <v>168.7</v>
       </c>
       <c r="D100" t="n">
-        <v>0.3340000000000001</v>
+        <v>53.51763888888888</v>
       </c>
     </row>
     <row r="101">
@@ -1847,7 +1847,7 @@
         <v>168.5166666666667</v>
       </c>
       <c r="D101" t="n">
-        <v>0.3336666666666668</v>
+        <v>53.42791666666668</v>
       </c>
     </row>
     <row r="102">
@@ -1861,7 +1861,7 @@
         <v>168.3333333333334</v>
       </c>
       <c r="D102" t="n">
-        <v>0.3333333333333335</v>
+        <v>53.33819444444444</v>
       </c>
     </row>
     <row r="103">
@@ -1875,7 +1875,7 @@
         <v>168.15</v>
       </c>
       <c r="D103" t="n">
-        <v>0.3330000000000001</v>
+        <v>53.24847222222223</v>
       </c>
     </row>
     <row r="104">
@@ -1889,7 +1889,7 @@
         <v>167.9666666666667</v>
       </c>
       <c r="D104" t="n">
-        <v>0.3326666666666668</v>
+        <v>53.15875</v>
       </c>
     </row>
     <row r="105">
@@ -1903,7 +1903,7 @@
         <v>167.7833333333334</v>
       </c>
       <c r="D105" t="n">
-        <v>0.3323333333333335</v>
+        <v>53.06902777777776</v>
       </c>
     </row>
     <row r="106">
@@ -1917,7 +1917,7 @@
         <v>167.6</v>
       </c>
       <c r="D106" t="n">
-        <v>0.3320000000000001</v>
+        <v>52.97930555555556</v>
       </c>
     </row>
     <row r="107">
@@ -1931,7 +1931,7 @@
         <v>167.4166666666667</v>
       </c>
       <c r="D107" t="n">
-        <v>0.3316666666666668</v>
+        <v>52.88958333333332</v>
       </c>
     </row>
     <row r="108">
@@ -1945,7 +1945,7 @@
         <v>167.2333333333333</v>
       </c>
       <c r="D108" t="n">
-        <v>0.3313333333333335</v>
+        <v>52.79986111111111</v>
       </c>
     </row>
     <row r="109">
@@ -1959,7 +1959,7 @@
         <v>167.0500000000001</v>
       </c>
       <c r="D109" t="n">
-        <v>0.3310000000000001</v>
+        <v>52.71013888888888</v>
       </c>
     </row>
     <row r="110">
@@ -1973,7 +1973,7 @@
         <v>166.8666666666667</v>
       </c>
       <c r="D110" t="n">
-        <v>0.3306666666666668</v>
+        <v>52.62041666666667</v>
       </c>
     </row>
     <row r="111">
@@ -1987,7 +1987,7 @@
         <v>166.6833333333334</v>
       </c>
       <c r="D111" t="n">
-        <v>0.3303333333333335</v>
+        <v>52.53069444444444</v>
       </c>
     </row>
     <row r="112">
@@ -2001,7 +2001,7 @@
         <v>166.5000000000001</v>
       </c>
       <c r="D112" t="n">
-        <v>0.3300000000000001</v>
+        <v>52.44097222222223</v>
       </c>
     </row>
     <row r="113">
@@ -2015,7 +2015,7 @@
         <v>166.3166666666667</v>
       </c>
       <c r="D113" t="n">
-        <v>0.3296666666666668</v>
+        <v>52.35124999999999</v>
       </c>
     </row>
     <row r="114">
@@ -2029,7 +2029,7 @@
         <v>166.1333333333334</v>
       </c>
       <c r="D114" t="n">
-        <v>0.3293333333333335</v>
+        <v>52.26152777777779</v>
       </c>
     </row>
     <row r="115">
@@ -2043,7 +2043,7 @@
         <v>165.95</v>
       </c>
       <c r="D115" t="n">
-        <v>0.3290000000000001</v>
+        <v>52.17180555555555</v>
       </c>
     </row>
     <row r="116">
@@ -2057,7 +2057,7 @@
         <v>165.7666666666667</v>
       </c>
       <c r="D116" t="n">
-        <v>0.3286666666666668</v>
+        <v>52.08208333333334</v>
       </c>
     </row>
     <row r="117">
@@ -2071,7 +2071,7 @@
         <v>165.5833333333334</v>
       </c>
       <c r="D117" t="n">
-        <v>0.3283333333333335</v>
+        <v>51.99236111111111</v>
       </c>
     </row>
     <row r="118">
@@ -2085,7 +2085,7 @@
         <v>165.4</v>
       </c>
       <c r="D118" t="n">
-        <v>0.3280000000000001</v>
+        <v>51.9026388888889</v>
       </c>
     </row>
     <row r="119">
@@ -2099,7 +2099,7 @@
         <v>165.2166666666667</v>
       </c>
       <c r="D119" t="n">
-        <v>0.3276666666666668</v>
+        <v>51.81291666666667</v>
       </c>
     </row>
     <row r="120">
@@ -2113,7 +2113,7 @@
         <v>165.0333333333334</v>
       </c>
       <c r="D120" t="n">
-        <v>0.3273333333333335</v>
+        <v>51.72319444444443</v>
       </c>
     </row>
     <row r="121">
@@ -2127,7 +2127,7 @@
         <v>164.85</v>
       </c>
       <c r="D121" t="n">
-        <v>0.3270000000000001</v>
+        <v>51.63347222222222</v>
       </c>
     </row>
     <row r="122">
@@ -2141,7 +2141,7 @@
         <v>164.6666666666667</v>
       </c>
       <c r="D122" t="n">
-        <v>0.3266666666666668</v>
+        <v>51.54374999999999</v>
       </c>
     </row>
     <row r="123">
@@ -2155,7 +2155,7 @@
         <v>164.4833333333334</v>
       </c>
       <c r="D123" t="n">
-        <v>0.3263333333333335</v>
+        <v>51.45402777777778</v>
       </c>
     </row>
     <row r="124">
@@ -2169,7 +2169,7 @@
         <v>164.3000000000001</v>
       </c>
       <c r="D124" t="n">
-        <v>0.3260000000000001</v>
+        <v>51.36430555555555</v>
       </c>
     </row>
     <row r="125">
@@ -2183,7 +2183,7 @@
         <v>164.1166666666667</v>
       </c>
       <c r="D125" t="n">
-        <v>0.3256666666666668</v>
+        <v>51.27458333333334</v>
       </c>
     </row>
     <row r="126">
@@ -2197,7 +2197,7 @@
         <v>163.9333333333334</v>
       </c>
       <c r="D126" t="n">
-        <v>0.3253333333333335</v>
+        <v>51.1848611111111</v>
       </c>
     </row>
     <row r="127">
@@ -2211,7 +2211,7 @@
         <v>163.7500000000001</v>
       </c>
       <c r="D127" t="n">
-        <v>0.3250000000000001</v>
+        <v>51.0951388888889</v>
       </c>
     </row>
     <row r="128">
@@ -2225,7 +2225,7 @@
         <v>163.5666666666667</v>
       </c>
       <c r="D128" t="n">
-        <v>0.3246666666666668</v>
+        <v>51.00541666666666</v>
       </c>
     </row>
     <row r="129">
@@ -2239,7 +2239,7 @@
         <v>163.3833333333334</v>
       </c>
       <c r="D129" t="n">
-        <v>0.3243333333333335</v>
+        <v>50.91569444444445</v>
       </c>
     </row>
     <row r="130">
@@ -2253,7 +2253,7 @@
         <v>163.2</v>
       </c>
       <c r="D130" t="n">
-        <v>0.3240000000000001</v>
+        <v>50.82597222222222</v>
       </c>
     </row>
     <row r="131">
@@ -2267,7 +2267,7 @@
         <v>163.0166666666667</v>
       </c>
       <c r="D131" t="n">
-        <v>0.3236666666666668</v>
+        <v>50.73625000000001</v>
       </c>
     </row>
     <row r="132">
@@ -2281,7 +2281,7 @@
         <v>162.8333333333334</v>
       </c>
       <c r="D132" t="n">
-        <v>0.3233333333333335</v>
+        <v>50.64652777777778</v>
       </c>
     </row>
     <row r="133">
@@ -2295,7 +2295,7 @@
         <v>162.65</v>
       </c>
       <c r="D133" t="n">
-        <v>0.3230000000000001</v>
+        <v>50.55680555555554</v>
       </c>
     </row>
     <row r="134">
@@ -2309,7 +2309,7 @@
         <v>162.4666666666667</v>
       </c>
       <c r="D134" t="n">
-        <v>0.3226666666666668</v>
+        <v>50.46708333333333</v>
       </c>
     </row>
     <row r="135">
@@ -2323,7 +2323,7 @@
         <v>162.2833333333334</v>
       </c>
       <c r="D135" t="n">
-        <v>0.3223333333333335</v>
+        <v>50.3773611111111</v>
       </c>
     </row>
     <row r="136">
@@ -2337,7 +2337,7 @@
         <v>162.1</v>
       </c>
       <c r="D136" t="n">
-        <v>0.3220000000000001</v>
+        <v>50.28763888888889</v>
       </c>
     </row>
     <row r="137">
@@ -2351,7 +2351,7 @@
         <v>161.9166666666667</v>
       </c>
       <c r="D137" t="n">
-        <v>0.3216666666666668</v>
+        <v>50.19791666666666</v>
       </c>
     </row>
     <row r="138">
@@ -2365,7 +2365,7 @@
         <v>161.7333333333334</v>
       </c>
       <c r="D138" t="n">
-        <v>0.3213333333333335</v>
+        <v>50.10819444444445</v>
       </c>
     </row>
     <row r="139">
@@ -2379,7 +2379,7 @@
         <v>161.5500000000001</v>
       </c>
       <c r="D139" t="n">
-        <v>0.3210000000000001</v>
+        <v>50.01847222222221</v>
       </c>
     </row>
     <row r="140">
@@ -2393,7 +2393,7 @@
         <v>161.3666666666667</v>
       </c>
       <c r="D140" t="n">
-        <v>0.3206666666666668</v>
+        <v>49.92875000000001</v>
       </c>
     </row>
     <row r="141">
@@ -2407,7 +2407,7 @@
         <v>161.1833333333334</v>
       </c>
       <c r="D141" t="n">
-        <v>0.3203333333333335</v>
+        <v>49.83902777777777</v>
       </c>
     </row>
     <row r="142">
@@ -2421,7 +2421,7 @@
         <v>161.0000000000001</v>
       </c>
       <c r="D142" t="n">
-        <v>0.3200000000000001</v>
+        <v>49.74930555555557</v>
       </c>
     </row>
     <row r="143">
@@ -2435,7 +2435,7 @@
         <v>160.8166666666667</v>
       </c>
       <c r="D143" t="n">
-        <v>0.3196666666666668</v>
+        <v>49.65958333333333</v>
       </c>
     </row>
     <row r="144">
@@ -2449,7 +2449,7 @@
         <v>160.6333333333334</v>
       </c>
       <c r="D144" t="n">
-        <v>0.3193333333333335</v>
+        <v>49.56986111111112</v>
       </c>
     </row>
     <row r="145">
@@ -2463,7 +2463,7 @@
         <v>160.45</v>
       </c>
       <c r="D145" t="n">
-        <v>0.3190000000000001</v>
+        <v>49.48013888888889</v>
       </c>
     </row>
     <row r="146">
@@ -2477,7 +2477,7 @@
         <v>160.2666666666667</v>
       </c>
       <c r="D146" t="n">
-        <v>0.3186666666666668</v>
+        <v>49.39041666666668</v>
       </c>
     </row>
     <row r="147">
@@ -2491,7 +2491,7 @@
         <v>160.0833333333334</v>
       </c>
       <c r="D147" t="n">
-        <v>0.3183333333333335</v>
+        <v>49.30069444444445</v>
       </c>
     </row>
     <row r="148">
@@ -2505,7 +2505,7 @@
         <v>159.9</v>
       </c>
       <c r="D148" t="n">
-        <v>0.3180000000000001</v>
+        <v>49.21097222222221</v>
       </c>
     </row>
     <row r="149">
@@ -2519,7 +2519,7 @@
         <v>159.7166666666667</v>
       </c>
       <c r="D149" t="n">
-        <v>0.3176666666666668</v>
+        <v>49.12125</v>
       </c>
     </row>
     <row r="150">
@@ -2533,7 +2533,7 @@
         <v>159.5333333333334</v>
       </c>
       <c r="D150" t="n">
-        <v>0.3173333333333335</v>
+        <v>49.03152777777777</v>
       </c>
     </row>
     <row r="151">
@@ -2547,7 +2547,7 @@
         <v>159.3500000000001</v>
       </c>
       <c r="D151" t="n">
-        <v>0.3170000000000001</v>
+        <v>48.94180555555556</v>
       </c>
     </row>
     <row r="152">
@@ -2561,7 +2561,7 @@
         <v>159.1666666666667</v>
       </c>
       <c r="D152" t="n">
-        <v>0.3166666666666668</v>
+        <v>48.85208333333333</v>
       </c>
     </row>
     <row r="153">
@@ -2575,7 +2575,7 @@
         <v>158.9833333333334</v>
       </c>
       <c r="D153" t="n">
-        <v>0.3163333333333335</v>
+        <v>48.76236111111112</v>
       </c>
     </row>
     <row r="154">
@@ -2589,7 +2589,7 @@
         <v>158.8000000000001</v>
       </c>
       <c r="D154" t="n">
-        <v>0.3160000000000001</v>
+        <v>48.67263888888888</v>
       </c>
     </row>
     <row r="155">
@@ -2603,7 +2603,7 @@
         <v>158.6166666666667</v>
       </c>
       <c r="D155" t="n">
-        <v>0.3156666666666668</v>
+        <v>48.58291666666668</v>
       </c>
     </row>
     <row r="156">
@@ -2617,7 +2617,7 @@
         <v>158.4333333333334</v>
       </c>
       <c r="D156" t="n">
-        <v>0.3153333333333335</v>
+        <v>48.49319444444444</v>
       </c>
     </row>
     <row r="157">
@@ -2631,7 +2631,7 @@
         <v>158.2500000000001</v>
       </c>
       <c r="D157" t="n">
-        <v>0.3150000000000001</v>
+        <v>48.40347222222223</v>
       </c>
     </row>
     <row r="158">
@@ -2645,7 +2645,7 @@
         <v>158.0666666666667</v>
       </c>
       <c r="D158" t="n">
-        <v>0.3146666666666668</v>
+        <v>48.31375</v>
       </c>
     </row>
     <row r="159">
@@ -2659,7 +2659,7 @@
         <v>157.8833333333334</v>
       </c>
       <c r="D159" t="n">
-        <v>0.3143333333333335</v>
+        <v>48.22402777777779</v>
       </c>
     </row>
     <row r="160">
@@ -2673,7 +2673,7 @@
         <v>157.7</v>
       </c>
       <c r="D160" t="n">
-        <v>0.3140000000000001</v>
+        <v>48.13430555555556</v>
       </c>
     </row>
     <row r="161">
@@ -2687,7 +2687,7 @@
         <v>157.5166666666667</v>
       </c>
       <c r="D161" t="n">
-        <v>0.3136666666666668</v>
+        <v>48.04458333333335</v>
       </c>
     </row>
     <row r="162">
@@ -2701,7 +2701,7 @@
         <v>157.3333333333334</v>
       </c>
       <c r="D162" t="n">
-        <v>0.3133333333333335</v>
+        <v>47.95486111111111</v>
       </c>
     </row>
     <row r="163">
@@ -2715,7 +2715,7 @@
         <v>157.15</v>
       </c>
       <c r="D163" t="n">
-        <v>0.3130000000000001</v>
+        <v>47.86513888888888</v>
       </c>
     </row>
     <row r="164">
@@ -2729,7 +2729,7 @@
         <v>156.9666666666667</v>
       </c>
       <c r="D164" t="n">
-        <v>0.3126666666666668</v>
+        <v>47.77541666666667</v>
       </c>
     </row>
     <row r="165">
@@ -2743,7 +2743,7 @@
         <v>156.7833333333334</v>
       </c>
       <c r="D165" t="n">
-        <v>0.3123333333333335</v>
+        <v>47.68569444444444</v>
       </c>
     </row>
     <row r="166">
@@ -2757,7 +2757,7 @@
         <v>156.6000000000001</v>
       </c>
       <c r="D166" t="n">
-        <v>0.3120000000000001</v>
+        <v>47.59597222222223</v>
       </c>
     </row>
     <row r="167">
@@ -2771,7 +2771,7 @@
         <v>156.4166666666667</v>
       </c>
       <c r="D167" t="n">
-        <v>0.3116666666666668</v>
+        <v>47.50624999999999</v>
       </c>
     </row>
     <row r="168">
@@ -2785,7 +2785,7 @@
         <v>156.2333333333334</v>
       </c>
       <c r="D168" t="n">
-        <v>0.3113333333333335</v>
+        <v>47.41652777777779</v>
       </c>
     </row>
     <row r="169">
@@ -2799,7 +2799,7 @@
         <v>156.0500000000001</v>
       </c>
       <c r="D169" t="n">
-        <v>0.3110000000000001</v>
+        <v>47.32680555555555</v>
       </c>
     </row>
     <row r="170">
@@ -2813,7 +2813,7 @@
         <v>155.8666666666667</v>
       </c>
       <c r="D170" t="n">
-        <v>0.3106666666666668</v>
+        <v>47.23708333333335</v>
       </c>
     </row>
     <row r="171">
@@ -2827,7 +2827,7 @@
         <v>155.6833333333334</v>
       </c>
       <c r="D171" t="n">
-        <v>0.3103333333333335</v>
+        <v>47.14736111111111</v>
       </c>
     </row>
     <row r="172">
@@ -2841,7 +2841,7 @@
         <v>155.5000000000001</v>
       </c>
       <c r="D172" t="n">
-        <v>0.3100000000000001</v>
+        <v>47.0576388888889</v>
       </c>
     </row>
     <row r="173">
@@ -2855,7 +2855,7 @@
         <v>155.3166666666667</v>
       </c>
       <c r="D173" t="n">
-        <v>0.3096666666666668</v>
+        <v>46.96791666666667</v>
       </c>
     </row>
     <row r="174">
@@ -2869,7 +2869,7 @@
         <v>155.1333333333334</v>
       </c>
       <c r="D174" t="n">
-        <v>0.3093333333333335</v>
+        <v>46.87819444444446</v>
       </c>
     </row>
     <row r="175">
@@ -2883,7 +2883,7 @@
         <v>154.95</v>
       </c>
       <c r="D175" t="n">
-        <v>0.3090000000000002</v>
+        <v>46.78847222222223</v>
       </c>
     </row>
     <row r="176">
@@ -2897,7 +2897,7 @@
         <v>154.7666666666667</v>
       </c>
       <c r="D176" t="n">
-        <v>0.3086666666666668</v>
+        <v>46.69874999999999</v>
       </c>
     </row>
     <row r="177">
@@ -2911,7 +2911,7 @@
         <v>154.5833333333334</v>
       </c>
       <c r="D177" t="n">
-        <v>0.3083333333333335</v>
+        <v>46.60902777777778</v>
       </c>
     </row>
     <row r="178">
@@ -2925,7 +2925,7 @@
         <v>154.4</v>
       </c>
       <c r="D178" t="n">
-        <v>0.3080000000000002</v>
+        <v>46.51930555555555</v>
       </c>
     </row>
     <row r="179">
@@ -2939,7 +2939,7 @@
         <v>154.2166666666668</v>
       </c>
       <c r="D179" t="n">
-        <v>0.3076666666666668</v>
+        <v>46.42958333333334</v>
       </c>
     </row>
     <row r="180">
@@ -2953,7 +2953,7 @@
         <v>154.0333333333334</v>
       </c>
       <c r="D180" t="n">
-        <v>0.3073333333333335</v>
+        <v>46.33986111111111</v>
       </c>
     </row>
     <row r="181">
@@ -2967,7 +2967,7 @@
         <v>153.8500000000001</v>
       </c>
       <c r="D181" t="n">
-        <v>0.3070000000000002</v>
+        <v>46.2501388888889</v>
       </c>
     </row>
     <row r="182">
@@ -2981,7 +2981,7 @@
         <v>153.6666666666667</v>
       </c>
       <c r="D182" t="n">
-        <v>0.3066666666666668</v>
+        <v>46.16041666666666</v>
       </c>
     </row>
     <row r="183">
@@ -2995,7 +2995,7 @@
         <v>153.4833333333334</v>
       </c>
       <c r="D183" t="n">
-        <v>0.3063333333333335</v>
+        <v>46.07069444444446</v>
       </c>
     </row>
     <row r="184">
@@ -3009,7 +3009,7 @@
         <v>153.3000000000001</v>
       </c>
       <c r="D184" t="n">
-        <v>0.3060000000000002</v>
+        <v>45.98097222222222</v>
       </c>
     </row>
     <row r="185">
@@ -3023,7 +3023,7 @@
         <v>153.1166666666667</v>
       </c>
       <c r="D185" t="n">
-        <v>0.3056666666666668</v>
+        <v>45.89125000000001</v>
       </c>
     </row>
     <row r="186">
@@ -3037,7 +3037,7 @@
         <v>152.9333333333334</v>
       </c>
       <c r="D186" t="n">
-        <v>0.3053333333333335</v>
+        <v>45.80152777777778</v>
       </c>
     </row>
     <row r="187">
@@ -3051,7 +3051,7 @@
         <v>152.7500000000001</v>
       </c>
       <c r="D187" t="n">
-        <v>0.3050000000000002</v>
+        <v>45.71180555555557</v>
       </c>
     </row>
     <row r="188">
@@ -3065,7 +3065,7 @@
         <v>152.5666666666667</v>
       </c>
       <c r="D188" t="n">
-        <v>0.3046666666666668</v>
+        <v>45.62208333333334</v>
       </c>
     </row>
     <row r="189">
@@ -3079,7 +3079,7 @@
         <v>152.3833333333334</v>
       </c>
       <c r="D189" t="n">
-        <v>0.3043333333333335</v>
+        <v>45.53236111111113</v>
       </c>
     </row>
     <row r="190">
@@ -3093,7 +3093,7 @@
         <v>152.2</v>
       </c>
       <c r="D190" t="n">
-        <v>0.3040000000000002</v>
+        <v>45.44263888888889</v>
       </c>
     </row>
     <row r="191">
@@ -3107,7 +3107,7 @@
         <v>152.0166666666667</v>
       </c>
       <c r="D191" t="n">
-        <v>0.3036666666666668</v>
+        <v>45.35291666666666</v>
       </c>
     </row>
     <row r="192">
@@ -3121,7 +3121,7 @@
         <v>151.8333333333334</v>
       </c>
       <c r="D192" t="n">
-        <v>0.3033333333333335</v>
+        <v>45.26319444444445</v>
       </c>
     </row>
     <row r="193">
@@ -3135,7 +3135,7 @@
         <v>151.6500000000001</v>
       </c>
       <c r="D193" t="n">
-        <v>0.3030000000000002</v>
+        <v>45.17347222222222</v>
       </c>
     </row>
     <row r="194">
@@ -3149,7 +3149,7 @@
         <v>151.4666666666668</v>
       </c>
       <c r="D194" t="n">
-        <v>0.3026666666666668</v>
+        <v>45.08375000000001</v>
       </c>
     </row>
     <row r="195">
@@ -3163,7 +3163,7 @@
         <v>151.2833333333334</v>
       </c>
       <c r="D195" t="n">
-        <v>0.3023333333333335</v>
+        <v>44.99402777777777</v>
       </c>
     </row>
     <row r="196">
@@ -3177,7 +3177,7 @@
         <v>151.1000000000001</v>
       </c>
       <c r="D196" t="n">
-        <v>0.3020000000000002</v>
+        <v>44.90430555555557</v>
       </c>
     </row>
     <row r="197">
@@ -3191,7 +3191,7 @@
         <v>150.9166666666667</v>
       </c>
       <c r="D197" t="n">
-        <v>0.3016666666666667</v>
+        <v>44.81458333333333</v>
       </c>
     </row>
     <row r="198">
@@ -3205,7 +3205,7 @@
         <v>150.7333333333334</v>
       </c>
       <c r="D198" t="n">
-        <v>0.3013333333333335</v>
+        <v>44.72486111111112</v>
       </c>
     </row>
     <row r="199">
@@ -3219,7 +3219,7 @@
         <v>150.5500000000001</v>
       </c>
       <c r="D199" t="n">
-        <v>0.3010000000000002</v>
+        <v>44.63513888888889</v>
       </c>
     </row>
     <row r="200">
@@ -3233,7 +3233,7 @@
         <v>150.3666666666667</v>
       </c>
       <c r="D200" t="n">
-        <v>0.3006666666666667</v>
+        <v>44.54541666666668</v>
       </c>
     </row>
     <row r="201">
@@ -3247,7 +3247,7 @@
         <v>150.1833333333334</v>
       </c>
       <c r="D201" t="n">
-        <v>0.3003333333333335</v>
+        <v>44.45569444444445</v>
       </c>
     </row>
     <row r="202">
@@ -3261,7 +3261,7 @@
         <v>150</v>
       </c>
       <c r="D202" t="n">
-        <v>0.3</v>
+        <v>45</v>
       </c>
     </row>
     <row r="203">
@@ -3275,7 +3275,7 @@
         <v>149.8166666666667</v>
       </c>
       <c r="D203" t="n">
-        <v>0.2996666666666666</v>
+        <v>44.8950611111111</v>
       </c>
     </row>
     <row r="204">
@@ -3289,7 +3289,7 @@
         <v>149.6333333333333</v>
       </c>
       <c r="D204" t="n">
-        <v>0.2993333333333333</v>
+        <v>44.79024444444444</v>
       </c>
     </row>
     <row r="205">
@@ -3303,7 +3303,7 @@
         <v>149.45</v>
       </c>
       <c r="D205" t="n">
-        <v>0.299</v>
+        <v>44.68554999999999</v>
       </c>
     </row>
     <row r="206">
@@ -3317,7 +3317,7 @@
         <v>149.2666666666667</v>
       </c>
       <c r="D206" t="n">
-        <v>0.2986666666666666</v>
+        <v>44.58097777777778</v>
       </c>
     </row>
     <row r="207">
@@ -3331,7 +3331,7 @@
         <v>149.0833333333333</v>
       </c>
       <c r="D207" t="n">
-        <v>0.2983333333333333</v>
+        <v>44.47652777777778</v>
       </c>
     </row>
     <row r="208">
@@ -3345,7 +3345,7 @@
         <v>148.9</v>
       </c>
       <c r="D208" t="n">
-        <v>0.298</v>
+        <v>44.3722</v>
       </c>
     </row>
     <row r="209">
@@ -3359,7 +3359,7 @@
         <v>148.7166666666667</v>
       </c>
       <c r="D209" t="n">
-        <v>0.2976666666666666</v>
+        <v>44.26799444444444</v>
       </c>
     </row>
     <row r="210">
@@ -3373,7 +3373,7 @@
         <v>148.5333333333333</v>
       </c>
       <c r="D210" t="n">
-        <v>0.2973333333333333</v>
+        <v>44.16391111111111</v>
       </c>
     </row>
     <row r="211">
@@ -3387,7 +3387,7 @@
         <v>148.35</v>
       </c>
       <c r="D211" t="n">
-        <v>0.297</v>
+        <v>44.05994999999999</v>
       </c>
     </row>
     <row r="212">
@@ -3401,7 +3401,7 @@
         <v>148.1666666666667</v>
       </c>
       <c r="D212" t="n">
-        <v>0.2966666666666666</v>
+        <v>43.95611111111111</v>
       </c>
     </row>
     <row r="213">
@@ -3415,7 +3415,7 @@
         <v>147.9833333333333</v>
       </c>
       <c r="D213" t="n">
-        <v>0.2963333333333333</v>
+        <v>43.85239444444445</v>
       </c>
     </row>
     <row r="214">
@@ -3429,7 +3429,7 @@
         <v>147.8</v>
       </c>
       <c r="D214" t="n">
-        <v>0.296</v>
+        <v>43.7488</v>
       </c>
     </row>
     <row r="215">
@@ -3443,7 +3443,7 @@
         <v>147.6166666666667</v>
       </c>
       <c r="D215" t="n">
-        <v>0.2956666666666666</v>
+        <v>43.64532777777777</v>
       </c>
     </row>
     <row r="216">
@@ -3457,7 +3457,7 @@
         <v>147.4333333333333</v>
       </c>
       <c r="D216" t="n">
-        <v>0.2953333333333333</v>
+        <v>43.54197777777778</v>
       </c>
     </row>
     <row r="217">
@@ -3471,7 +3471,7 @@
         <v>147.25</v>
       </c>
       <c r="D217" t="n">
-        <v>0.295</v>
+        <v>43.43875</v>
       </c>
     </row>
     <row r="218">
@@ -3485,7 +3485,7 @@
         <v>147.0666666666667</v>
       </c>
       <c r="D218" t="n">
-        <v>0.2946666666666667</v>
+        <v>43.33564444444445</v>
       </c>
     </row>
     <row r="219">
@@ -3499,7 +3499,7 @@
         <v>146.8833333333333</v>
       </c>
       <c r="D219" t="n">
-        <v>0.2943333333333333</v>
+        <v>43.23266111111111</v>
       </c>
     </row>
     <row r="220">
@@ -3513,7 +3513,7 @@
         <v>146.7</v>
       </c>
       <c r="D220" t="n">
-        <v>0.294</v>
+        <v>43.1298</v>
       </c>
     </row>
     <row r="221">
@@ -3527,7 +3527,7 @@
         <v>146.5166666666667</v>
       </c>
       <c r="D221" t="n">
-        <v>0.2936666666666667</v>
+        <v>43.02706111111112</v>
       </c>
     </row>
     <row r="222">
@@ -3541,7 +3541,7 @@
         <v>146.3333333333333</v>
       </c>
       <c r="D222" t="n">
-        <v>0.2933333333333333</v>
+        <v>42.92444444444445</v>
       </c>
     </row>
     <row r="223">
@@ -3555,7 +3555,7 @@
         <v>146.15</v>
       </c>
       <c r="D223" t="n">
-        <v>0.293</v>
+        <v>42.82195</v>
       </c>
     </row>
     <row r="224">
@@ -3569,7 +3569,7 @@
         <v>145.9666666666667</v>
       </c>
       <c r="D224" t="n">
-        <v>0.2926666666666667</v>
+        <v>42.71957777777778</v>
       </c>
     </row>
     <row r="225">
@@ -3583,7 +3583,7 @@
         <v>145.7833333333333</v>
       </c>
       <c r="D225" t="n">
-        <v>0.2923333333333333</v>
+        <v>42.61732777777777</v>
       </c>
     </row>
     <row r="226">
@@ -3597,7 +3597,7 @@
         <v>145.6</v>
       </c>
       <c r="D226" t="n">
-        <v>0.292</v>
+        <v>42.51520000000001</v>
       </c>
     </row>
     <row r="227">
@@ -3611,7 +3611,7 @@
         <v>145.4166666666667</v>
       </c>
       <c r="D227" t="n">
-        <v>0.2916666666666667</v>
+        <v>42.41319444444445</v>
       </c>
     </row>
     <row r="228">
@@ -3625,7 +3625,7 @@
         <v>145.2333333333333</v>
       </c>
       <c r="D228" t="n">
-        <v>0.2913333333333333</v>
+        <v>42.31131111111112</v>
       </c>
     </row>
     <row r="229">
@@ -3639,7 +3639,7 @@
         <v>145.05</v>
       </c>
       <c r="D229" t="n">
-        <v>0.291</v>
+        <v>42.20955</v>
       </c>
     </row>
     <row r="230">
@@ -3653,7 +3653,7 @@
         <v>144.8666666666667</v>
       </c>
       <c r="D230" t="n">
-        <v>0.2906666666666667</v>
+        <v>42.10791111111111</v>
       </c>
     </row>
     <row r="231">
@@ -3667,7 +3667,7 @@
         <v>144.6833333333333</v>
       </c>
       <c r="D231" t="n">
-        <v>0.2903333333333333</v>
+        <v>42.00639444444445</v>
       </c>
     </row>
     <row r="232">
@@ -3681,7 +3681,7 @@
         <v>144.5</v>
       </c>
       <c r="D232" t="n">
-        <v>0.29</v>
+        <v>41.90499999999999</v>
       </c>
     </row>
     <row r="233">
@@ -3695,7 +3695,7 @@
         <v>144.3166666666667</v>
       </c>
       <c r="D233" t="n">
-        <v>0.2896666666666667</v>
+        <v>41.80372777777778</v>
       </c>
     </row>
     <row r="234">
@@ -3709,7 +3709,7 @@
         <v>144.1333333333334</v>
       </c>
       <c r="D234" t="n">
-        <v>0.2893333333333333</v>
+        <v>41.70257777777778</v>
       </c>
     </row>
     <row r="235">
@@ -3723,7 +3723,7 @@
         <v>143.95</v>
       </c>
       <c r="D235" t="n">
-        <v>0.289</v>
+        <v>41.60155</v>
       </c>
     </row>
     <row r="236">
@@ -3737,7 +3737,7 @@
         <v>143.7666666666667</v>
       </c>
       <c r="D236" t="n">
-        <v>0.2886666666666667</v>
+        <v>41.50064444444445</v>
       </c>
     </row>
     <row r="237">
@@ -3751,7 +3751,7 @@
         <v>143.5833333333333</v>
       </c>
       <c r="D237" t="n">
-        <v>0.2883333333333333</v>
+        <v>41.39986111111111</v>
       </c>
     </row>
     <row r="238">
@@ -3765,7 +3765,7 @@
         <v>143.4</v>
       </c>
       <c r="D238" t="n">
-        <v>0.288</v>
+        <v>41.2992</v>
       </c>
     </row>
     <row r="239">
@@ -3779,7 +3779,7 @@
         <v>143.2166666666667</v>
       </c>
       <c r="D239" t="n">
-        <v>0.2876666666666667</v>
+        <v>41.19866111111111</v>
       </c>
     </row>
     <row r="240">
@@ -3793,7 +3793,7 @@
         <v>143.0333333333334</v>
       </c>
       <c r="D240" t="n">
-        <v>0.2873333333333333</v>
+        <v>41.09824444444445</v>
       </c>
     </row>
     <row r="241">
@@ -3807,7 +3807,7 @@
         <v>142.85</v>
       </c>
       <c r="D241" t="n">
-        <v>0.287</v>
+        <v>40.99795</v>
       </c>
     </row>
     <row r="242">
@@ -3821,7 +3821,7 @@
         <v>142.6666666666667</v>
       </c>
       <c r="D242" t="n">
-        <v>0.2866666666666667</v>
+        <v>40.89777777777778</v>
       </c>
     </row>
     <row r="243">
@@ -3835,7 +3835,7 @@
         <v>142.4833333333333</v>
       </c>
       <c r="D243" t="n">
-        <v>0.2863333333333333</v>
+        <v>40.79772777777778</v>
       </c>
     </row>
     <row r="244">
@@ -3849,7 +3849,7 @@
         <v>142.3</v>
       </c>
       <c r="D244" t="n">
-        <v>0.286</v>
+        <v>40.6978</v>
       </c>
     </row>
     <row r="245">
@@ -3863,7 +3863,7 @@
         <v>142.1166666666667</v>
       </c>
       <c r="D245" t="n">
-        <v>0.2856666666666667</v>
+        <v>40.59799444444445</v>
       </c>
     </row>
     <row r="246">
@@ -3877,7 +3877,7 @@
         <v>141.9333333333333</v>
       </c>
       <c r="D246" t="n">
-        <v>0.2853333333333333</v>
+        <v>40.49831111111111</v>
       </c>
     </row>
     <row r="247">
@@ -3891,7 +3891,7 @@
         <v>141.75</v>
       </c>
       <c r="D247" t="n">
-        <v>0.285</v>
+        <v>40.39875000000001</v>
       </c>
     </row>
     <row r="248">
@@ -3905,7 +3905,7 @@
         <v>141.5666666666667</v>
       </c>
       <c r="D248" t="n">
-        <v>0.2846666666666667</v>
+        <v>40.29931111111112</v>
       </c>
     </row>
     <row r="249">
@@ -3919,7 +3919,7 @@
         <v>141.3833333333334</v>
       </c>
       <c r="D249" t="n">
-        <v>0.2843333333333333</v>
+        <v>40.19999444444445</v>
       </c>
     </row>
     <row r="250">
@@ -3933,7 +3933,7 @@
         <v>141.2</v>
       </c>
       <c r="D250" t="n">
-        <v>0.284</v>
+        <v>40.10080000000001</v>
       </c>
     </row>
     <row r="251">
@@ -3947,7 +3947,7 @@
         <v>141.0166666666667</v>
       </c>
       <c r="D251" t="n">
-        <v>0.2836666666666667</v>
+        <v>40.00172777777778</v>
       </c>
     </row>
     <row r="252">
@@ -3961,7 +3961,7 @@
         <v>140.8333333333333</v>
       </c>
       <c r="D252" t="n">
-        <v>0.2833333333333333</v>
+        <v>39.90277777777778</v>
       </c>
     </row>
     <row r="253">
@@ -3975,7 +3975,7 @@
         <v>140.65</v>
       </c>
       <c r="D253" t="n">
-        <v>0.283</v>
+        <v>39.80395000000001</v>
       </c>
     </row>
     <row r="254">
@@ -3989,7 +3989,7 @@
         <v>140.4666666666667</v>
       </c>
       <c r="D254" t="n">
-        <v>0.2826666666666667</v>
+        <v>39.70524444444445</v>
       </c>
     </row>
     <row r="255">
@@ -4003,7 +4003,7 @@
         <v>140.2833333333334</v>
       </c>
       <c r="D255" t="n">
-        <v>0.2823333333333333</v>
+        <v>39.60666111111112</v>
       </c>
     </row>
     <row r="256">
@@ -4017,7 +4017,7 @@
         <v>140.1</v>
       </c>
       <c r="D256" t="n">
-        <v>0.282</v>
+        <v>39.50820000000001</v>
       </c>
     </row>
     <row r="257">
@@ -4031,7 +4031,7 @@
         <v>139.9166666666667</v>
       </c>
       <c r="D257" t="n">
-        <v>0.2816666666666667</v>
+        <v>39.40986111111112</v>
       </c>
     </row>
     <row r="258">
@@ -4045,7 +4045,7 @@
         <v>139.7333333333333</v>
       </c>
       <c r="D258" t="n">
-        <v>0.2813333333333333</v>
+        <v>39.31164444444445</v>
       </c>
     </row>
     <row r="259">
@@ -4059,7 +4059,7 @@
         <v>139.55</v>
       </c>
       <c r="D259" t="n">
-        <v>0.281</v>
+        <v>39.21355000000001</v>
       </c>
     </row>
     <row r="260">
@@ -4073,7 +4073,7 @@
         <v>139.3666666666667</v>
       </c>
       <c r="D260" t="n">
-        <v>0.2806666666666667</v>
+        <v>39.11557777777778</v>
       </c>
     </row>
     <row r="261">
@@ -4087,7 +4087,7 @@
         <v>139.1833333333334</v>
       </c>
       <c r="D261" t="n">
-        <v>0.2803333333333333</v>
+        <v>39.01772777777779</v>
       </c>
     </row>
     <row r="262">
@@ -4101,7 +4101,7 @@
         <v>139</v>
       </c>
       <c r="D262" t="n">
-        <v>0.28</v>
+        <v>38.92000000000001</v>
       </c>
     </row>
     <row r="263">
@@ -4115,7 +4115,7 @@
         <v>138.8166666666667</v>
       </c>
       <c r="D263" t="n">
-        <v>0.2796666666666667</v>
+        <v>38.82239444444446</v>
       </c>
     </row>
     <row r="264">
@@ -4129,7 +4129,7 @@
         <v>138.6333333333334</v>
       </c>
       <c r="D264" t="n">
-        <v>0.2793333333333333</v>
+        <v>38.72491111111111</v>
       </c>
     </row>
     <row r="265">
@@ -4143,7 +4143,7 @@
         <v>138.45</v>
       </c>
       <c r="D265" t="n">
-        <v>0.279</v>
+        <v>38.62755000000001</v>
       </c>
     </row>
     <row r="266">
@@ -4157,7 +4157,7 @@
         <v>138.2666666666667</v>
       </c>
       <c r="D266" t="n">
-        <v>0.2786666666666667</v>
+        <v>38.53031111111112</v>
       </c>
     </row>
     <row r="267">
@@ -4171,7 +4171,7 @@
         <v>138.0833333333333</v>
       </c>
       <c r="D267" t="n">
-        <v>0.2783333333333333</v>
+        <v>38.43319444444445</v>
       </c>
     </row>
     <row r="268">
@@ -4185,7 +4185,7 @@
         <v>137.9</v>
       </c>
       <c r="D268" t="n">
-        <v>0.278</v>
+        <v>38.33620000000001</v>
       </c>
     </row>
     <row r="269">
@@ -4199,7 +4199,7 @@
         <v>137.7166666666667</v>
       </c>
       <c r="D269" t="n">
-        <v>0.2776666666666667</v>
+        <v>38.23932777777779</v>
       </c>
     </row>
     <row r="270">
@@ -4213,7 +4213,7 @@
         <v>137.5333333333334</v>
       </c>
       <c r="D270" t="n">
-        <v>0.2773333333333333</v>
+        <v>38.14257777777778</v>
       </c>
     </row>
     <row r="271">
@@ -4227,7 +4227,7 @@
         <v>137.35</v>
       </c>
       <c r="D271" t="n">
-        <v>0.277</v>
+        <v>38.04595000000001</v>
       </c>
     </row>
     <row r="272">
@@ -4241,7 +4241,7 @@
         <v>137.1666666666667</v>
       </c>
       <c r="D272" t="n">
-        <v>0.2766666666666667</v>
+        <v>37.94944444444445</v>
       </c>
     </row>
     <row r="273">
@@ -4255,7 +4255,7 @@
         <v>136.9833333333333</v>
       </c>
       <c r="D273" t="n">
-        <v>0.2763333333333333</v>
+        <v>37.85306111111111</v>
       </c>
     </row>
     <row r="274">
@@ -4269,7 +4269,7 @@
         <v>136.8</v>
       </c>
       <c r="D274" t="n">
-        <v>0.276</v>
+        <v>37.75680000000001</v>
       </c>
     </row>
     <row r="275">
@@ -4283,7 +4283,7 @@
         <v>136.6166666666667</v>
       </c>
       <c r="D275" t="n">
-        <v>0.2756666666666667</v>
+        <v>37.66066111111112</v>
       </c>
     </row>
     <row r="276">
@@ -4297,7 +4297,7 @@
         <v>136.4333333333334</v>
       </c>
       <c r="D276" t="n">
-        <v>0.2753333333333333</v>
+        <v>37.56464444444445</v>
       </c>
     </row>
     <row r="277">
@@ -4311,7 +4311,7 @@
         <v>136.25</v>
       </c>
       <c r="D277" t="n">
-        <v>0.275</v>
+        <v>37.46875000000001</v>
       </c>
     </row>
     <row r="278">
@@ -4325,7 +4325,7 @@
         <v>136.0666666666667</v>
       </c>
       <c r="D278" t="n">
-        <v>0.2746666666666667</v>
+        <v>37.37297777777778</v>
       </c>
     </row>
     <row r="279">
@@ -4339,7 +4339,7 @@
         <v>135.8833333333334</v>
       </c>
       <c r="D279" t="n">
-        <v>0.2743333333333334</v>
+        <v>37.27732777777779</v>
       </c>
     </row>
     <row r="280">
@@ -4353,7 +4353,7 @@
         <v>135.7</v>
       </c>
       <c r="D280" t="n">
-        <v>0.274</v>
+        <v>37.18180000000001</v>
       </c>
     </row>
     <row r="281">
@@ -4367,7 +4367,7 @@
         <v>135.5166666666667</v>
       </c>
       <c r="D281" t="n">
-        <v>0.2736666666666667</v>
+        <v>37.08639444444446</v>
       </c>
     </row>
     <row r="282">
@@ -4381,7 +4381,7 @@
         <v>135.3333333333334</v>
       </c>
       <c r="D282" t="n">
-        <v>0.2733333333333334</v>
+        <v>36.99111111111112</v>
       </c>
     </row>
     <row r="283">
@@ -4395,7 +4395,7 @@
         <v>135.15</v>
       </c>
       <c r="D283" t="n">
-        <v>0.273</v>
+        <v>36.89595000000001</v>
       </c>
     </row>
     <row r="284">
@@ -4409,7 +4409,7 @@
         <v>134.9666666666667</v>
       </c>
       <c r="D284" t="n">
-        <v>0.2726666666666667</v>
+        <v>36.80091111111112</v>
       </c>
     </row>
     <row r="285">
@@ -4423,7 +4423,7 @@
         <v>134.7833333333334</v>
       </c>
       <c r="D285" t="n">
-        <v>0.2723333333333334</v>
+        <v>36.70599444444446</v>
       </c>
     </row>
     <row r="286">
@@ -4437,7 +4437,7 @@
         <v>134.6</v>
       </c>
       <c r="D286" t="n">
-        <v>0.272</v>
+        <v>36.61120000000001</v>
       </c>
     </row>
     <row r="287">
@@ -4451,7 +4451,7 @@
         <v>134.4166666666667</v>
       </c>
       <c r="D287" t="n">
-        <v>0.2716666666666667</v>
+        <v>36.51652777777778</v>
       </c>
     </row>
     <row r="288">
@@ -4465,7 +4465,7 @@
         <v>134.2333333333333</v>
       </c>
       <c r="D288" t="n">
-        <v>0.2713333333333334</v>
+        <v>36.42197777777778</v>
       </c>
     </row>
     <row r="289">
@@ -4479,7 +4479,7 @@
         <v>134.05</v>
       </c>
       <c r="D289" t="n">
-        <v>0.271</v>
+        <v>36.32755000000002</v>
       </c>
     </row>
     <row r="290">
@@ -4493,7 +4493,7 @@
         <v>133.8666666666667</v>
       </c>
       <c r="D290" t="n">
-        <v>0.2706666666666667</v>
+        <v>36.23324444444445</v>
       </c>
     </row>
     <row r="291">
@@ -4507,7 +4507,7 @@
         <v>133.6833333333334</v>
       </c>
       <c r="D291" t="n">
-        <v>0.2703333333333334</v>
+        <v>36.13906111111113</v>
       </c>
     </row>
     <row r="292">
@@ -4521,7 +4521,7 @@
         <v>133.5</v>
       </c>
       <c r="D292" t="n">
-        <v>0.27</v>
+        <v>36.04500000000001</v>
       </c>
     </row>
     <row r="293">
@@ -4535,7 +4535,7 @@
         <v>133.3166666666667</v>
       </c>
       <c r="D293" t="n">
-        <v>0.2696666666666667</v>
+        <v>35.95106111111112</v>
       </c>
     </row>
     <row r="294">
@@ -4549,7 +4549,7 @@
         <v>133.1333333333334</v>
       </c>
       <c r="D294" t="n">
-        <v>0.2693333333333334</v>
+        <v>35.85724444444445</v>
       </c>
     </row>
     <row r="295">
@@ -4563,7 +4563,7 @@
         <v>132.95</v>
       </c>
       <c r="D295" t="n">
-        <v>0.269</v>
+        <v>35.76355000000002</v>
       </c>
     </row>
     <row r="296">
@@ -4577,7 +4577,7 @@
         <v>132.7666666666667</v>
       </c>
       <c r="D296" t="n">
-        <v>0.2686666666666667</v>
+        <v>35.66997777777779</v>
       </c>
     </row>
     <row r="297">
@@ -4591,7 +4591,7 @@
         <v>132.5833333333334</v>
       </c>
       <c r="D297" t="n">
-        <v>0.2683333333333334</v>
+        <v>35.57652777777779</v>
       </c>
     </row>
     <row r="298">
@@ -4605,7 +4605,7 @@
         <v>132.4</v>
       </c>
       <c r="D298" t="n">
-        <v>0.268</v>
+        <v>35.48320000000001</v>
       </c>
     </row>
     <row r="299">
@@ -4619,7 +4619,7 @@
         <v>132.2166666666667</v>
       </c>
       <c r="D299" t="n">
-        <v>0.2676666666666667</v>
+        <v>35.38999444444446</v>
       </c>
     </row>
     <row r="300">
@@ -4633,7 +4633,7 @@
         <v>132.0333333333334</v>
       </c>
       <c r="D300" t="n">
-        <v>0.2673333333333334</v>
+        <v>35.29691111111112</v>
       </c>
     </row>
     <row r="301">
@@ -4647,7 +4647,7 @@
         <v>131.85</v>
       </c>
       <c r="D301" t="n">
-        <v>0.267</v>
+        <v>35.20395000000001</v>
       </c>
     </row>
     <row r="302">
@@ -4661,7 +4661,7 @@
         <v>131.6666666666667</v>
       </c>
       <c r="D302" t="n">
-        <v>0.2666666666666667</v>
+        <v>35.11111111111112</v>
       </c>
     </row>
     <row r="303">
@@ -4675,7 +4675,7 @@
         <v>131.4833333333334</v>
       </c>
       <c r="D303" t="n">
-        <v>0.2663333333333334</v>
+        <v>35.01839444444446</v>
       </c>
     </row>
     <row r="304">
@@ -4689,7 +4689,7 @@
         <v>131.3</v>
       </c>
       <c r="D304" t="n">
-        <v>0.266</v>
+        <v>34.92580000000001</v>
       </c>
     </row>
     <row r="305">
@@ -4703,7 +4703,7 @@
         <v>131.1166666666667</v>
       </c>
       <c r="D305" t="n">
-        <v>0.2656666666666667</v>
+        <v>34.8333277777778</v>
       </c>
     </row>
     <row r="306">
@@ -4717,7 +4717,7 @@
         <v>130.9333333333334</v>
       </c>
       <c r="D306" t="n">
-        <v>0.2653333333333334</v>
+        <v>34.74097777777779</v>
       </c>
     </row>
     <row r="307">
@@ -4731,7 +4731,7 @@
         <v>130.75</v>
       </c>
       <c r="D307" t="n">
-        <v>0.265</v>
+        <v>34.64875000000001</v>
       </c>
     </row>
     <row r="308">
@@ -4745,7 +4745,7 @@
         <v>130.5666666666667</v>
       </c>
       <c r="D308" t="n">
-        <v>0.2646666666666667</v>
+        <v>34.55664444444446</v>
       </c>
     </row>
     <row r="309">
@@ -4759,7 +4759,7 @@
         <v>130.3833333333334</v>
       </c>
       <c r="D309" t="n">
-        <v>0.2643333333333334</v>
+        <v>34.46466111111113</v>
       </c>
     </row>
     <row r="310">
@@ -4773,7 +4773,7 @@
         <v>130.2</v>
       </c>
       <c r="D310" t="n">
-        <v>0.264</v>
+        <v>34.37280000000001</v>
       </c>
     </row>
     <row r="311">
@@ -4787,7 +4787,7 @@
         <v>130.0166666666667</v>
       </c>
       <c r="D311" t="n">
-        <v>0.2636666666666667</v>
+        <v>34.28106111111113</v>
       </c>
     </row>
     <row r="312">
@@ -4801,7 +4801,7 @@
         <v>129.8333333333334</v>
       </c>
       <c r="D312" t="n">
-        <v>0.2633333333333334</v>
+        <v>34.18944444444446</v>
       </c>
     </row>
     <row r="313">
@@ -4815,7 +4815,7 @@
         <v>129.65</v>
       </c>
       <c r="D313" t="n">
-        <v>0.263</v>
+        <v>34.09795000000001</v>
       </c>
     </row>
     <row r="314">
@@ -4829,7 +4829,7 @@
         <v>129.4666666666667</v>
       </c>
       <c r="D314" t="n">
-        <v>0.2626666666666667</v>
+        <v>34.00657777777779</v>
       </c>
     </row>
     <row r="315">
@@ -4843,7 +4843,7 @@
         <v>129.2833333333334</v>
       </c>
       <c r="D315" t="n">
-        <v>0.2623333333333334</v>
+        <v>33.91532777777779</v>
       </c>
     </row>
     <row r="316">
@@ -4857,7 +4857,7 @@
         <v>129.1000000000001</v>
       </c>
       <c r="D316" t="n">
-        <v>0.262</v>
+        <v>33.82420000000001</v>
       </c>
     </row>
     <row r="317">
@@ -4871,7 +4871,7 @@
         <v>128.9166666666667</v>
       </c>
       <c r="D317" t="n">
-        <v>0.2616666666666667</v>
+        <v>33.73319444444446</v>
       </c>
     </row>
     <row r="318">
@@ -4885,7 +4885,7 @@
         <v>128.7333333333334</v>
       </c>
       <c r="D318" t="n">
-        <v>0.2613333333333334</v>
+        <v>33.64231111111113</v>
       </c>
     </row>
     <row r="319">
@@ -4899,7 +4899,7 @@
         <v>128.55</v>
       </c>
       <c r="D319" t="n">
-        <v>0.261</v>
+        <v>33.55155000000001</v>
       </c>
     </row>
     <row r="320">
@@ -4913,7 +4913,7 @@
         <v>128.3666666666667</v>
       </c>
       <c r="D320" t="n">
-        <v>0.2606666666666667</v>
+        <v>33.46091111111112</v>
       </c>
     </row>
     <row r="321">
@@ -4927,7 +4927,7 @@
         <v>128.1833333333334</v>
       </c>
       <c r="D321" t="n">
-        <v>0.2603333333333334</v>
+        <v>33.37039444444446</v>
       </c>
     </row>
     <row r="322">
@@ -4941,7 +4941,7 @@
         <v>128.0000000000001</v>
       </c>
       <c r="D322" t="n">
-        <v>0.26</v>
+        <v>33.28000000000002</v>
       </c>
     </row>
     <row r="323">
@@ -4955,7 +4955,7 @@
         <v>127.8166666666667</v>
       </c>
       <c r="D323" t="n">
-        <v>0.2596666666666667</v>
+        <v>33.18972777777779</v>
       </c>
     </row>
     <row r="324">
@@ -4969,7 +4969,7 @@
         <v>127.6333333333334</v>
       </c>
       <c r="D324" t="n">
-        <v>0.2593333333333334</v>
+        <v>33.0995777777778</v>
       </c>
     </row>
     <row r="325">
@@ -4983,7 +4983,7 @@
         <v>127.45</v>
       </c>
       <c r="D325" t="n">
-        <v>0.259</v>
+        <v>33.00955000000001</v>
       </c>
     </row>
     <row r="326">
@@ -4997,7 +4997,7 @@
         <v>127.2666666666667</v>
       </c>
       <c r="D326" t="n">
-        <v>0.2586666666666667</v>
+        <v>32.91964444444446</v>
       </c>
     </row>
     <row r="327">
@@ -5011,7 +5011,7 @@
         <v>127.0833333333334</v>
       </c>
       <c r="D327" t="n">
-        <v>0.2583333333333334</v>
+        <v>32.82986111111112</v>
       </c>
     </row>
     <row r="328">
@@ -5025,7 +5025,7 @@
         <v>126.9</v>
       </c>
       <c r="D328" t="n">
-        <v>0.258</v>
+        <v>32.74020000000002</v>
       </c>
     </row>
     <row r="329">
@@ -5039,7 +5039,7 @@
         <v>126.7166666666667</v>
       </c>
       <c r="D329" t="n">
-        <v>0.2576666666666667</v>
+        <v>32.65066111111113</v>
       </c>
     </row>
     <row r="330">
@@ -5053,7 +5053,7 @@
         <v>126.5333333333334</v>
       </c>
       <c r="D330" t="n">
-        <v>0.2573333333333334</v>
+        <v>32.56124444444445</v>
       </c>
     </row>
     <row r="331">
@@ -5067,7 +5067,7 @@
         <v>126.3500000000001</v>
       </c>
       <c r="D331" t="n">
-        <v>0.257</v>
+        <v>32.47195000000001</v>
       </c>
     </row>
     <row r="332">
@@ -5081,7 +5081,7 @@
         <v>126.1666666666667</v>
       </c>
       <c r="D332" t="n">
-        <v>0.2566666666666667</v>
+        <v>32.3827777777778</v>
       </c>
     </row>
     <row r="333">
@@ -5095,7 +5095,7 @@
         <v>125.9833333333334</v>
       </c>
       <c r="D333" t="n">
-        <v>0.2563333333333334</v>
+        <v>32.29372777777779</v>
       </c>
     </row>
     <row r="334">
@@ -5109,7 +5109,7 @@
         <v>125.8</v>
       </c>
       <c r="D334" t="n">
-        <v>0.256</v>
+        <v>32.20480000000001</v>
       </c>
     </row>
     <row r="335">
@@ -5123,7 +5123,7 @@
         <v>125.6166666666667</v>
       </c>
       <c r="D335" t="n">
-        <v>0.2556666666666667</v>
+        <v>32.11599444444446</v>
       </c>
     </row>
     <row r="336">
@@ -5137,7 +5137,7 @@
         <v>125.4333333333334</v>
       </c>
       <c r="D336" t="n">
-        <v>0.2553333333333334</v>
+        <v>32.02731111111112</v>
       </c>
     </row>
     <row r="337">
@@ -5151,7 +5151,7 @@
         <v>125.25</v>
       </c>
       <c r="D337" t="n">
-        <v>0.255</v>
+        <v>31.93875000000001</v>
       </c>
     </row>
     <row r="338">
@@ -5165,7 +5165,7 @@
         <v>125.0666666666667</v>
       </c>
       <c r="D338" t="n">
-        <v>0.2546666666666667</v>
+        <v>31.85031111111113</v>
       </c>
     </row>
     <row r="339">
@@ -5179,7 +5179,7 @@
         <v>124.8833333333334</v>
       </c>
       <c r="D339" t="n">
-        <v>0.2543333333333334</v>
+        <v>31.76199444444446</v>
       </c>
     </row>
     <row r="340">
@@ -5193,7 +5193,7 @@
         <v>124.7</v>
       </c>
       <c r="D340" t="n">
-        <v>0.2540000000000001</v>
+        <v>31.67380000000002</v>
       </c>
     </row>
     <row r="341">
@@ -5207,7 +5207,7 @@
         <v>124.5166666666667</v>
       </c>
       <c r="D341" t="n">
-        <v>0.2536666666666667</v>
+        <v>31.58572777777779</v>
       </c>
     </row>
     <row r="342">
@@ -5221,7 +5221,7 @@
         <v>124.3333333333334</v>
       </c>
       <c r="D342" t="n">
-        <v>0.2533333333333334</v>
+        <v>31.4977777777778</v>
       </c>
     </row>
     <row r="343">
@@ -5235,7 +5235,7 @@
         <v>124.15</v>
       </c>
       <c r="D343" t="n">
-        <v>0.2530000000000001</v>
+        <v>31.40995000000002</v>
       </c>
     </row>
     <row r="344">
@@ -5249,7 +5249,7 @@
         <v>123.9666666666667</v>
       </c>
       <c r="D344" t="n">
-        <v>0.2526666666666667</v>
+        <v>31.32224444444446</v>
       </c>
     </row>
     <row r="345">
@@ -5263,7 +5263,7 @@
         <v>123.7833333333334</v>
       </c>
       <c r="D345" t="n">
-        <v>0.2523333333333334</v>
+        <v>31.23466111111113</v>
       </c>
     </row>
     <row r="346">
@@ -5277,7 +5277,7 @@
         <v>123.6000000000001</v>
       </c>
       <c r="D346" t="n">
-        <v>0.2520000000000001</v>
+        <v>31.14720000000002</v>
       </c>
     </row>
     <row r="347">
@@ -5291,7 +5291,7 @@
         <v>123.4166666666667</v>
       </c>
       <c r="D347" t="n">
-        <v>0.2516666666666667</v>
+        <v>31.05986111111113</v>
       </c>
     </row>
     <row r="348">
@@ -5305,7 +5305,7 @@
         <v>123.2333333333334</v>
       </c>
       <c r="D348" t="n">
-        <v>0.2513333333333334</v>
+        <v>30.97264444444446</v>
       </c>
     </row>
     <row r="349">
@@ -5319,7 +5319,7 @@
         <v>123.0500000000001</v>
       </c>
       <c r="D349" t="n">
-        <v>0.2510000000000001</v>
+        <v>30.88555000000002</v>
       </c>
     </row>
     <row r="350">
@@ -5333,7 +5333,7 @@
         <v>122.8666666666667</v>
       </c>
       <c r="D350" t="n">
-        <v>0.2506666666666667</v>
+        <v>30.79857777777779</v>
       </c>
     </row>
     <row r="351">
@@ -5347,7 +5347,7 @@
         <v>122.6833333333334</v>
       </c>
       <c r="D351" t="n">
-        <v>0.2503333333333334</v>
+        <v>30.71172777777779</v>
       </c>
     </row>
     <row r="352">
@@ -5361,7 +5361,7 @@
         <v>122.5000000000001</v>
       </c>
       <c r="D352" t="n">
-        <v>0.2500000000000001</v>
+        <v>30.62500000000002</v>
       </c>
     </row>
     <row r="353">
@@ -5375,7 +5375,7 @@
         <v>122.3166666666667</v>
       </c>
       <c r="D353" t="n">
-        <v>0.2496666666666667</v>
+        <v>30.53839444444446</v>
       </c>
     </row>
     <row r="354">
@@ -5389,7 +5389,7 @@
         <v>122.1333333333334</v>
       </c>
       <c r="D354" t="n">
-        <v>0.2493333333333334</v>
+        <v>30.45191111111113</v>
       </c>
     </row>
     <row r="355">
@@ -5403,7 +5403,7 @@
         <v>121.95</v>
       </c>
       <c r="D355" t="n">
-        <v>0.2490000000000001</v>
+        <v>30.36555000000002</v>
       </c>
     </row>
     <row r="356">
@@ -5417,7 +5417,7 @@
         <v>121.7666666666667</v>
       </c>
       <c r="D356" t="n">
-        <v>0.2486666666666667</v>
+        <v>30.27931111111113</v>
       </c>
     </row>
     <row r="357">
@@ -5431,7 +5431,7 @@
         <v>121.5833333333334</v>
       </c>
       <c r="D357" t="n">
-        <v>0.2483333333333334</v>
+        <v>30.19319444444446</v>
       </c>
     </row>
     <row r="358">
@@ -5445,7 +5445,7 @@
         <v>121.4000000000001</v>
       </c>
       <c r="D358" t="n">
-        <v>0.2480000000000001</v>
+        <v>30.10720000000002</v>
       </c>
     </row>
     <row r="359">
@@ -5459,7 +5459,7 @@
         <v>121.2166666666667</v>
       </c>
       <c r="D359" t="n">
-        <v>0.2476666666666667</v>
+        <v>30.0213277777778</v>
       </c>
     </row>
     <row r="360">
@@ -5473,7 +5473,7 @@
         <v>121.0333333333334</v>
       </c>
       <c r="D360" t="n">
-        <v>0.2473333333333334</v>
+        <v>29.9355777777778</v>
       </c>
     </row>
     <row r="361">
@@ -5487,7 +5487,7 @@
         <v>120.8500000000001</v>
       </c>
       <c r="D361" t="n">
-        <v>0.2470000000000001</v>
+        <v>29.84995000000002</v>
       </c>
     </row>
     <row r="362">
@@ -5501,7 +5501,7 @@
         <v>120.6666666666667</v>
       </c>
       <c r="D362" t="n">
-        <v>0.2466666666666667</v>
+        <v>29.76444444444446</v>
       </c>
     </row>
     <row r="363">
@@ -5515,7 +5515,7 @@
         <v>120.4833333333334</v>
       </c>
       <c r="D363" t="n">
-        <v>0.2463333333333334</v>
+        <v>29.67906111111113</v>
       </c>
     </row>
     <row r="364">
@@ -5529,7 +5529,7 @@
         <v>120.3000000000001</v>
       </c>
       <c r="D364" t="n">
-        <v>0.2460000000000001</v>
+        <v>29.59380000000002</v>
       </c>
     </row>
     <row r="365">
@@ -5543,7 +5543,7 @@
         <v>120.1166666666667</v>
       </c>
       <c r="D365" t="n">
-        <v>0.2456666666666667</v>
+        <v>29.50866111111113</v>
       </c>
     </row>
     <row r="366">
@@ -5557,7 +5557,7 @@
         <v>119.9333333333334</v>
       </c>
       <c r="D366" t="n">
-        <v>0.2453333333333334</v>
+        <v>29.42364444444446</v>
       </c>
     </row>
     <row r="367">
@@ -5571,7 +5571,7 @@
         <v>119.7500000000001</v>
       </c>
       <c r="D367" t="n">
-        <v>0.2450000000000001</v>
+        <v>29.33875000000002</v>
       </c>
     </row>
     <row r="368">
@@ -5585,7 +5585,7 @@
         <v>119.5666666666667</v>
       </c>
       <c r="D368" t="n">
-        <v>0.2446666666666667</v>
+        <v>29.25397777777779</v>
       </c>
     </row>
     <row r="369">
@@ -5599,7 +5599,7 @@
         <v>119.3833333333334</v>
       </c>
       <c r="D369" t="n">
-        <v>0.2443333333333334</v>
+        <v>29.1693277777778</v>
       </c>
     </row>
     <row r="370">
@@ -5613,7 +5613,7 @@
         <v>119.2000000000001</v>
       </c>
       <c r="D370" t="n">
-        <v>0.2440000000000001</v>
+        <v>29.08480000000002</v>
       </c>
     </row>
     <row r="371">
@@ -5627,7 +5627,7 @@
         <v>119.0166666666667</v>
       </c>
       <c r="D371" t="n">
-        <v>0.2436666666666667</v>
+        <v>29.00039444444446</v>
       </c>
     </row>
     <row r="372">
@@ -5641,7 +5641,7 @@
         <v>118.8333333333334</v>
       </c>
       <c r="D372" t="n">
-        <v>0.2433333333333334</v>
+        <v>28.91611111111113</v>
       </c>
     </row>
     <row r="373">
@@ -5655,7 +5655,7 @@
         <v>118.6500000000001</v>
       </c>
       <c r="D373" t="n">
-        <v>0.243</v>
+        <v>28.83195000000002</v>
       </c>
     </row>
     <row r="374">
@@ -5669,7 +5669,7 @@
         <v>118.4666666666667</v>
       </c>
       <c r="D374" t="n">
-        <v>0.2426666666666667</v>
+        <v>28.74791111111113</v>
       </c>
     </row>
     <row r="375">
@@ -5683,7 +5683,7 @@
         <v>118.2833333333334</v>
       </c>
       <c r="D375" t="n">
-        <v>0.2423333333333334</v>
+        <v>28.66399444444446</v>
       </c>
     </row>
     <row r="376">
@@ -5697,7 +5697,7 @@
         <v>118.1000000000001</v>
       </c>
       <c r="D376" t="n">
-        <v>0.242</v>
+        <v>28.58020000000002</v>
       </c>
     </row>
     <row r="377">
@@ -5711,7 +5711,7 @@
         <v>117.9166666666667</v>
       </c>
       <c r="D377" t="n">
-        <v>0.2416666666666667</v>
+        <v>28.4965277777778</v>
       </c>
     </row>
     <row r="378">
@@ -5725,7 +5725,7 @@
         <v>117.7333333333334</v>
       </c>
       <c r="D378" t="n">
-        <v>0.2413333333333334</v>
+        <v>28.4129777777778</v>
       </c>
     </row>
     <row r="379">
@@ -5739,7 +5739,7 @@
         <v>117.5500000000001</v>
       </c>
       <c r="D379" t="n">
-        <v>0.241</v>
+        <v>28.32955000000002</v>
       </c>
     </row>
     <row r="380">
@@ -5753,7 +5753,7 @@
         <v>117.3666666666667</v>
       </c>
       <c r="D380" t="n">
-        <v>0.2406666666666667</v>
+        <v>28.24624444444447</v>
       </c>
     </row>
     <row r="381">
@@ -5767,7 +5767,7 @@
         <v>117.1833333333334</v>
       </c>
       <c r="D381" t="n">
-        <v>0.2403333333333334</v>
+        <v>28.16306111111113</v>
       </c>
     </row>
     <row r="382">
@@ -5781,7 +5781,7 @@
         <v>117.0000000000001</v>
       </c>
       <c r="D382" t="n">
-        <v>0.24</v>
+        <v>28.08000000000002</v>
       </c>
     </row>
     <row r="383">
@@ -5795,7 +5795,7 @@
         <v>116.8166666666667</v>
       </c>
       <c r="D383" t="n">
-        <v>0.2396666666666667</v>
+        <v>27.99706111111113</v>
       </c>
     </row>
     <row r="384">
@@ -5809,7 +5809,7 @@
         <v>116.6333333333334</v>
       </c>
       <c r="D384" t="n">
-        <v>0.2393333333333334</v>
+        <v>27.91424444444447</v>
       </c>
     </row>
     <row r="385">
@@ -5823,7 +5823,7 @@
         <v>116.4500000000001</v>
       </c>
       <c r="D385" t="n">
-        <v>0.239</v>
+        <v>27.83155000000002</v>
       </c>
     </row>
     <row r="386">
@@ -5837,7 +5837,7 @@
         <v>116.2666666666667</v>
       </c>
       <c r="D386" t="n">
-        <v>0.2386666666666667</v>
+        <v>27.7489777777778</v>
       </c>
     </row>
     <row r="387">
@@ -5851,7 +5851,7 @@
         <v>116.0833333333334</v>
       </c>
       <c r="D387" t="n">
-        <v>0.2383333333333334</v>
+        <v>27.6665277777778</v>
       </c>
     </row>
     <row r="388">
@@ -5865,7 +5865,7 @@
         <v>115.9000000000001</v>
       </c>
       <c r="D388" t="n">
-        <v>0.238</v>
+        <v>27.58420000000002</v>
       </c>
     </row>
     <row r="389">
@@ -5879,7 +5879,7 @@
         <v>115.7166666666667</v>
       </c>
       <c r="D389" t="n">
-        <v>0.2376666666666667</v>
+        <v>27.50199444444446</v>
       </c>
     </row>
     <row r="390">
@@ -5893,7 +5893,7 @@
         <v>115.5333333333334</v>
       </c>
       <c r="D390" t="n">
-        <v>0.2373333333333334</v>
+        <v>27.41991111111113</v>
       </c>
     </row>
     <row r="391">
@@ -5907,7 +5907,7 @@
         <v>115.3500000000001</v>
       </c>
       <c r="D391" t="n">
-        <v>0.237</v>
+        <v>27.33795000000002</v>
       </c>
     </row>
     <row r="392">
@@ -5921,7 +5921,7 @@
         <v>115.1666666666667</v>
       </c>
       <c r="D392" t="n">
-        <v>0.2366666666666667</v>
+        <v>27.25611111111114</v>
       </c>
     </row>
     <row r="393">
@@ -5935,7 +5935,7 @@
         <v>114.9833333333334</v>
       </c>
       <c r="D393" t="n">
-        <v>0.2363333333333334</v>
+        <v>27.17439444444447</v>
       </c>
     </row>
     <row r="394">
@@ -5949,7 +5949,7 @@
         <v>114.8000000000001</v>
       </c>
       <c r="D394" t="n">
-        <v>0.236</v>
+        <v>27.09280000000002</v>
       </c>
     </row>
     <row r="395">
@@ -5963,7 +5963,7 @@
         <v>114.6166666666667</v>
       </c>
       <c r="D395" t="n">
-        <v>0.2356666666666667</v>
+        <v>27.0113277777778</v>
       </c>
     </row>
     <row r="396">
@@ -5977,7 +5977,7 @@
         <v>114.4333333333334</v>
       </c>
       <c r="D396" t="n">
-        <v>0.2353333333333334</v>
+        <v>26.9299777777778</v>
       </c>
     </row>
     <row r="397">
@@ -5991,7 +5991,7 @@
         <v>114.2500000000001</v>
       </c>
       <c r="D397" t="n">
-        <v>0.235</v>
+        <v>26.84875000000002</v>
       </c>
     </row>
     <row r="398">
@@ -6005,7 +6005,7 @@
         <v>114.0666666666667</v>
       </c>
       <c r="D398" t="n">
-        <v>0.2346666666666667</v>
+        <v>26.76764444444447</v>
       </c>
     </row>
     <row r="399">
@@ -6019,7 +6019,7 @@
         <v>113.8833333333334</v>
       </c>
       <c r="D399" t="n">
-        <v>0.2343333333333334</v>
+        <v>26.68666111111114</v>
       </c>
     </row>
     <row r="400">
@@ -6033,7 +6033,7 @@
         <v>113.7000000000001</v>
       </c>
       <c r="D400" t="n">
-        <v>0.234</v>
+        <v>26.60580000000002</v>
       </c>
     </row>
     <row r="401">
@@ -6047,7 +6047,7 @@
         <v>113.5166666666667</v>
       </c>
       <c r="D401" t="n">
-        <v>0.2336666666666667</v>
+        <v>26.52506111111113</v>
       </c>
     </row>
     <row r="402">
@@ -6061,7 +6061,7 @@
         <v>113.3333333333334</v>
       </c>
       <c r="D402" t="n">
-        <v>0.2333333333333334</v>
+        <v>26.44444444444447</v>
       </c>
     </row>
     <row r="403">
@@ -6075,7 +6075,7 @@
         <v>113.1500000000001</v>
       </c>
       <c r="D403" t="n">
-        <v>0.233</v>
+        <v>26.36395000000002</v>
       </c>
     </row>
     <row r="404">
@@ -6089,7 +6089,7 @@
         <v>112.9666666666667</v>
       </c>
       <c r="D404" t="n">
-        <v>0.2326666666666667</v>
+        <v>26.2835777777778</v>
       </c>
     </row>
     <row r="405">
@@ -6103,7 +6103,7 @@
         <v>112.7833333333334</v>
       </c>
       <c r="D405" t="n">
-        <v>0.2323333333333334</v>
+        <v>26.2033277777778</v>
       </c>
     </row>
     <row r="406">
@@ -6117,7 +6117,7 @@
         <v>112.6000000000001</v>
       </c>
       <c r="D406" t="n">
-        <v>0.232</v>
+        <v>26.12320000000002</v>
       </c>
     </row>
     <row r="407">
@@ -6131,7 +6131,7 @@
         <v>112.4166666666667</v>
       </c>
       <c r="D407" t="n">
-        <v>0.2316666666666667</v>
+        <v>26.04319444444447</v>
       </c>
     </row>
     <row r="408">
@@ -6145,7 +6145,7 @@
         <v>112.2333333333334</v>
       </c>
       <c r="D408" t="n">
-        <v>0.2313333333333334</v>
+        <v>25.96331111111114</v>
       </c>
     </row>
     <row r="409">
@@ -6159,7 +6159,7 @@
         <v>112.0500000000001</v>
       </c>
       <c r="D409" t="n">
-        <v>0.231</v>
+        <v>25.88355000000002</v>
       </c>
     </row>
     <row r="410">
@@ -6173,7 +6173,7 @@
         <v>111.8666666666667</v>
       </c>
       <c r="D410" t="n">
-        <v>0.2306666666666667</v>
+        <v>25.80391111111113</v>
       </c>
     </row>
     <row r="411">
@@ -6187,7 +6187,7 @@
         <v>111.6833333333334</v>
       </c>
       <c r="D411" t="n">
-        <v>0.2303333333333334</v>
+        <v>25.72439444444447</v>
       </c>
     </row>
     <row r="412">
@@ -6201,7 +6201,7 @@
         <v>111.5000000000001</v>
       </c>
       <c r="D412" t="n">
-        <v>0.2300000000000001</v>
+        <v>25.64500000000002</v>
       </c>
     </row>
     <row r="413">
@@ -6215,7 +6215,7 @@
         <v>111.3166666666667</v>
       </c>
       <c r="D413" t="n">
-        <v>0.2296666666666667</v>
+        <v>25.56572777777781</v>
       </c>
     </row>
     <row r="414">
@@ -6229,7 +6229,7 @@
         <v>111.1333333333334</v>
       </c>
       <c r="D414" t="n">
-        <v>0.2293333333333334</v>
+        <v>25.4865777777778</v>
       </c>
     </row>
     <row r="415">
@@ -6243,7 +6243,7 @@
         <v>110.9500000000001</v>
       </c>
       <c r="D415" t="n">
-        <v>0.2290000000000001</v>
+        <v>25.40755000000003</v>
       </c>
     </row>
     <row r="416">
@@ -6257,7 +6257,7 @@
         <v>110.7666666666667</v>
       </c>
       <c r="D416" t="n">
-        <v>0.2286666666666667</v>
+        <v>25.32864444444447</v>
       </c>
     </row>
     <row r="417">
@@ -6271,7 +6271,7 @@
         <v>110.5833333333334</v>
       </c>
       <c r="D417" t="n">
-        <v>0.2283333333333334</v>
+        <v>25.24986111111113</v>
       </c>
     </row>
     <row r="418">
@@ -6285,7 +6285,7 @@
         <v>110.4000000000001</v>
       </c>
       <c r="D418" t="n">
-        <v>0.2280000000000001</v>
+        <v>25.17120000000002</v>
       </c>
     </row>
     <row r="419">
@@ -6299,7 +6299,7 @@
         <v>110.2166666666667</v>
       </c>
       <c r="D419" t="n">
-        <v>0.2276666666666667</v>
+        <v>25.09266111111113</v>
       </c>
     </row>
     <row r="420">
@@ -6313,7 +6313,7 @@
         <v>110.0333333333334</v>
       </c>
       <c r="D420" t="n">
-        <v>0.2273333333333334</v>
+        <v>25.01424444444447</v>
       </c>
     </row>
     <row r="421">
@@ -6327,7 +6327,7 @@
         <v>109.8500000000001</v>
       </c>
       <c r="D421" t="n">
-        <v>0.2270000000000001</v>
+        <v>24.93595000000003</v>
       </c>
     </row>
     <row r="422">
@@ -6341,7 +6341,7 @@
         <v>109.6666666666667</v>
       </c>
       <c r="D422" t="n">
-        <v>0.2266666666666667</v>
+        <v>24.8577777777778</v>
       </c>
     </row>
     <row r="423">
@@ -6355,7 +6355,7 @@
         <v>109.4833333333334</v>
       </c>
       <c r="D423" t="n">
-        <v>0.2263333333333334</v>
+        <v>24.7797277777778</v>
       </c>
     </row>
     <row r="424">
@@ -6369,7 +6369,7 @@
         <v>109.3000000000001</v>
       </c>
       <c r="D424" t="n">
-        <v>0.2260000000000001</v>
+        <v>24.70180000000002</v>
       </c>
     </row>
     <row r="425">
@@ -6383,7 +6383,7 @@
         <v>109.1166666666667</v>
       </c>
       <c r="D425" t="n">
-        <v>0.2256666666666667</v>
+        <v>24.62399444444447</v>
       </c>
     </row>
     <row r="426">
@@ -6397,7 +6397,7 @@
         <v>108.9333333333334</v>
       </c>
       <c r="D426" t="n">
-        <v>0.2253333333333334</v>
+        <v>24.54631111111113</v>
       </c>
     </row>
     <row r="427">
@@ -6411,7 +6411,7 @@
         <v>108.7500000000001</v>
       </c>
       <c r="D427" t="n">
-        <v>0.2250000000000001</v>
+        <v>24.46875000000002</v>
       </c>
     </row>
     <row r="428">
@@ -6425,7 +6425,7 @@
         <v>108.5666666666667</v>
       </c>
       <c r="D428" t="n">
-        <v>0.2246666666666667</v>
+        <v>24.39131111111114</v>
       </c>
     </row>
     <row r="429">
@@ -6439,7 +6439,7 @@
         <v>108.3833333333334</v>
       </c>
       <c r="D429" t="n">
-        <v>0.2243333333333334</v>
+        <v>24.31399444444447</v>
       </c>
     </row>
     <row r="430">
@@ -6453,7 +6453,7 @@
         <v>108.2000000000001</v>
       </c>
       <c r="D430" t="n">
-        <v>0.2240000000000001</v>
+        <v>24.23680000000002</v>
       </c>
     </row>
     <row r="431">
@@ -6467,7 +6467,7 @@
         <v>108.0166666666667</v>
       </c>
       <c r="D431" t="n">
-        <v>0.2236666666666667</v>
+        <v>24.1597277777778</v>
       </c>
     </row>
     <row r="432">
@@ -6481,7 +6481,7 @@
         <v>107.8333333333334</v>
       </c>
       <c r="D432" t="n">
-        <v>0.2233333333333334</v>
+        <v>24.0827777777778</v>
       </c>
     </row>
     <row r="433">
@@ -6495,7 +6495,7 @@
         <v>107.6500000000001</v>
       </c>
       <c r="D433" t="n">
-        <v>0.2230000000000001</v>
+        <v>24.00595000000003</v>
       </c>
     </row>
     <row r="434">
@@ -6509,7 +6509,7 @@
         <v>107.4666666666668</v>
       </c>
       <c r="D434" t="n">
-        <v>0.2226666666666667</v>
+        <v>23.92924444444447</v>
       </c>
     </row>
     <row r="435">
@@ -6523,7 +6523,7 @@
         <v>107.2833333333334</v>
       </c>
       <c r="D435" t="n">
-        <v>0.2223333333333334</v>
+        <v>23.85266111111114</v>
       </c>
     </row>
     <row r="436">
@@ -6537,7 +6537,7 @@
         <v>107.1000000000001</v>
       </c>
       <c r="D436" t="n">
-        <v>0.2220000000000001</v>
+        <v>23.77620000000003</v>
       </c>
     </row>
     <row r="437">
@@ -6551,7 +6551,7 @@
         <v>106.9166666666667</v>
       </c>
       <c r="D437" t="n">
-        <v>0.2216666666666667</v>
+        <v>23.69986111111114</v>
       </c>
     </row>
     <row r="438">
@@ -6565,7 +6565,7 @@
         <v>106.7333333333334</v>
       </c>
       <c r="D438" t="n">
-        <v>0.2213333333333334</v>
+        <v>23.62364444444447</v>
       </c>
     </row>
     <row r="439">
@@ -6579,7 +6579,7 @@
         <v>106.5500000000001</v>
       </c>
       <c r="D439" t="n">
-        <v>0.2210000000000001</v>
+        <v>23.54755000000003</v>
       </c>
     </row>
     <row r="440">
@@ -6593,7 +6593,7 @@
         <v>106.3666666666668</v>
       </c>
       <c r="D440" t="n">
-        <v>0.2206666666666667</v>
+        <v>23.47157777777781</v>
       </c>
     </row>
     <row r="441">
@@ -6607,7 +6607,7 @@
         <v>106.1833333333334</v>
       </c>
       <c r="D441" t="n">
-        <v>0.2203333333333334</v>
+        <v>23.3957277777778</v>
       </c>
     </row>
     <row r="442">
@@ -6621,7 +6621,7 @@
         <v>106.0000000000001</v>
       </c>
       <c r="D442" t="n">
-        <v>0.2200000000000001</v>
+        <v>23.32000000000003</v>
       </c>
     </row>
     <row r="443">
@@ -6635,7 +6635,7 @@
         <v>105.8166666666667</v>
       </c>
       <c r="D443" t="n">
-        <v>0.2196666666666667</v>
+        <v>23.24439444444447</v>
       </c>
     </row>
     <row r="444">
@@ -6649,7 +6649,7 @@
         <v>105.6333333333334</v>
       </c>
       <c r="D444" t="n">
-        <v>0.2193333333333334</v>
+        <v>23.16891111111114</v>
       </c>
     </row>
     <row r="445">
@@ -6663,7 +6663,7 @@
         <v>105.4500000000001</v>
       </c>
       <c r="D445" t="n">
-        <v>0.2190000000000001</v>
+        <v>23.09355000000003</v>
       </c>
     </row>
     <row r="446">
@@ -6677,7 +6677,7 @@
         <v>105.2666666666668</v>
       </c>
       <c r="D446" t="n">
-        <v>0.2186666666666667</v>
+        <v>23.01831111111114</v>
       </c>
     </row>
     <row r="447">
@@ -6691,7 +6691,7 @@
         <v>105.0833333333334</v>
       </c>
       <c r="D447" t="n">
-        <v>0.2183333333333334</v>
+        <v>22.94319444444447</v>
       </c>
     </row>
     <row r="448">
@@ -6705,7 +6705,7 @@
         <v>104.9000000000001</v>
       </c>
       <c r="D448" t="n">
-        <v>0.2180000000000001</v>
+        <v>22.86820000000003</v>
       </c>
     </row>
     <row r="449">
@@ -6719,7 +6719,7 @@
         <v>104.7166666666668</v>
       </c>
       <c r="D449" t="n">
-        <v>0.2176666666666667</v>
+        <v>22.7933277777778</v>
       </c>
     </row>
     <row r="450">
@@ -6733,7 +6733,7 @@
         <v>104.5333333333334</v>
       </c>
       <c r="D450" t="n">
-        <v>0.2173333333333334</v>
+        <v>22.7185777777778</v>
       </c>
     </row>
     <row r="451">
@@ -6747,7 +6747,7 @@
         <v>104.3500000000001</v>
       </c>
       <c r="D451" t="n">
-        <v>0.2170000000000001</v>
+        <v>22.64395000000003</v>
       </c>
     </row>
     <row r="452">
@@ -6761,7 +6761,7 @@
         <v>104.1666666666668</v>
       </c>
       <c r="D452" t="n">
-        <v>0.2166666666666667</v>
+        <v>22.56944444444447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>